<commit_message>
Have developed technique for producing and saving new images with continuous corn and c/sb rotations mapped.
</commit_message>
<xml_diff>
--- a/CropScapeConversions.xlsx
+++ b/CropScapeConversions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23700" windowHeight="16420" tabRatio="500"/>
+    <workbookView xWindow="19900" yWindow="0" windowWidth="8000" windowHeight="16420" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="136">
   <si>
     <t>Corn</t>
   </si>
@@ -415,6 +415,18 @@
   </si>
   <si>
     <t>Description</t>
+  </si>
+  <si>
+    <t>Corn/Soybean Rotation</t>
+  </si>
+  <si>
+    <t>Developed/Mixed</t>
+  </si>
+  <si>
+    <t>Other corn rotation</t>
+  </si>
+  <si>
+    <t>Other inconsistent</t>
   </si>
 </sst>
 </file>
@@ -454,12 +466,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -488,9 +506,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -836,10 +855,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B256"/>
+  <dimension ref="A1:B259"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A229" workbookViewId="0">
+      <selection activeCell="B260" sqref="B260"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1715,6 +1734,9 @@
       <c r="A127">
         <v>125</v>
       </c>
+      <c r="B127" s="2" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="128" spans="1:2">
       <c r="A128">
@@ -2521,6 +2543,30 @@
       </c>
       <c r="B256" t="s">
         <v>66</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2">
+      <c r="A257">
+        <v>255</v>
+      </c>
+      <c r="B257" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2">
+      <c r="A258">
+        <v>256</v>
+      </c>
+      <c r="B258" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2">
+      <c r="A259">
+        <v>257</v>
+      </c>
+      <c r="B259" s="2" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
start of hierarchical clustering technique
</commit_message>
<xml_diff>
--- a/CropScapeConversions.xlsx
+++ b/CropScapeConversions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="17980" yWindow="0" windowWidth="10760" windowHeight="16500" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="16500" tabRatio="500" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
@@ -14,6 +14,7 @@
     <sheet name="Combined" sheetId="4" r:id="rId5"/>
     <sheet name="Groups" sheetId="5" r:id="rId6"/>
     <sheet name="Counties" sheetId="6" r:id="rId7"/>
+    <sheet name="Tips" sheetId="10" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Colors!$A$1:$K$256</definedName>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1375" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1402" uniqueCount="331">
   <si>
     <t>Corn</t>
   </si>
@@ -909,18 +910,6 @@
     <t>Other</t>
   </si>
   <si>
-    <t>Boundary</t>
-  </si>
-  <si>
-    <t>Continous Corn</t>
-  </si>
-  <si>
-    <t>Everything else</t>
-  </si>
-  <si>
-    <t>Other ag in rotation</t>
-  </si>
-  <si>
     <t>General ag use</t>
   </si>
   <si>
@@ -937,6 +926,102 @@
   </si>
   <si>
     <t>Other corn</t>
+  </si>
+  <si>
+    <t>Activity</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>Continuous Corn</t>
+  </si>
+  <si>
+    <t>Rotation Corn</t>
+  </si>
+  <si>
+    <t>391461</t>
+  </si>
+  <si>
+    <t>Other ag</t>
+  </si>
+  <si>
+    <t>436278</t>
+  </si>
+  <si>
+    <t>Non ag</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>I think that the correct answer to this question is "use the raster and </t>
+  </si>
+  <si>
+    <t>the dismo package". In fact, dismo has the possibility of "fitting" </t>
+  </si>
+  <si>
+    <t>Maxent models directly from R. </t>
+  </si>
+  <si>
+    <t>In any case, with raster package you can easily import ASC files (I </t>
+  </si>
+  <si>
+    <t>suppose one file for each species), join them in an stack object and </t>
+  </si>
+  <si>
+    <t>depending on the size of your maps (i.e. number of pixels) and your </t>
+  </si>
+  <si>
+    <t>favourite classification approach (e.g. hierarchical vs. non </t>
+  </si>
+  <si>
+    <t>hierarchical) select the appropriate functions/packages. For example, </t>
+  </si>
+  <si>
+    <t>package vegan has function vegedist that is very appropriate for </t>
+  </si>
+  <si>
+    <t>community data. You can use it to compute a distance matrix (based on </t>
+  </si>
+  <si>
+    <t>the species data) between the pixels of your map an then submit this </t>
+  </si>
+  <si>
+    <t>matrix to hclust to compute a classificatory tree. You can cut this tree </t>
+  </si>
+  <si>
+    <t>(with cutree) at the desired number of communities or dissimilarity and </t>
+  </si>
+  <si>
+    <t>create a new layer in your raster stack with the "number" of cluster </t>
+  </si>
+  <si>
+    <t>to which each pixel has been assigned that can eassily ploted as a </t>
+  </si>
+  <si>
+    <t>"community map" </t>
+  </si>
+  <si>
+    <t>If the number of pixels is large you can consider using function clara in </t>
+  </si>
+  <si>
+    <t>package cluster or a combination of clara for a subsample (i.e. training </t>
+  </si>
+  <si>
+    <t>data set) plus a nearest neughbour classifier (e.g. function knn1) </t>
+  </si>
+  <si>
+    <t>HTH, </t>
+  </si>
+  <si>
+    <t>Marcelino </t>
+  </si>
+  <si>
+    <t xml:space="preserve">this was from: </t>
+  </si>
+  <si>
+    <t>http://r-sig-geo.2731867.n2.nabble.com/Spatial-cluster-analysis-td7149074.html</t>
   </si>
 </sst>
 </file>
@@ -949,7 +1034,7 @@
     <numFmt numFmtId="166" formatCode="0.000000000000"/>
     <numFmt numFmtId="167" formatCode="0.000000000000000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -993,6 +1078,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1077,14 +1167,12 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="37">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -3409,10 +3497,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y374"/>
+  <dimension ref="A1:X374"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView topLeftCell="I1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3426,15 +3514,13 @@
     <col min="8" max="8" width="23.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.5" customWidth="1"/>
     <col min="10" max="10" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.33203125" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="18.6640625" hidden="1" customWidth="1"/>
-    <col min="13" max="14" width="19.1640625" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="19.1640625" customWidth="1"/>
-    <col min="17" max="17" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.6640625" customWidth="1"/>
+    <col min="12" max="14" width="19.1640625" customWidth="1"/>
+    <col min="16" max="16" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:19">
       <c r="A1" s="1" t="s">
         <v>130</v>
       </c>
@@ -3463,24 +3549,21 @@
         <v>131</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>290</v>
+        <v>277</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="O1" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="S1" s="13"/>
-      <c r="T1" s="13"/>
-    </row>
-    <row r="2" spans="1:20">
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
+    </row>
+    <row r="2" spans="1:19">
       <c r="A2">
         <v>0</v>
       </c>
@@ -3517,17 +3600,14 @@
       <c r="M2">
         <v>3961</v>
       </c>
-      <c r="N2">
+      <c r="N2" s="12">
         <v>3961</v>
       </c>
-      <c r="O2" s="12">
-        <v>3961</v>
-      </c>
-      <c r="Q2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:19">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3556,28 +3636,25 @@
         <v>0</v>
       </c>
       <c r="K3">
-        <v>488741</v>
+        <v>497851</v>
       </c>
       <c r="L3">
-        <v>497851</v>
+        <v>502566</v>
       </c>
       <c r="M3">
-        <v>502566</v>
-      </c>
-      <c r="N3">
         <v>452347</v>
       </c>
-      <c r="O3" s="12">
+      <c r="N3" s="12">
         <v>109345</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="P3" t="s">
         <v>250</v>
       </c>
-      <c r="R3">
+      <c r="Q3">
         <v>640</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:19">
       <c r="A4">
         <v>5</v>
       </c>
@@ -3606,28 +3683,25 @@
         <v>92</v>
       </c>
       <c r="K4">
-        <v>5396</v>
+        <v>6367</v>
       </c>
       <c r="L4">
-        <v>6367</v>
+        <v>3725</v>
       </c>
       <c r="M4">
-        <v>3725</v>
-      </c>
-      <c r="N4">
         <v>2274</v>
       </c>
-      <c r="O4" s="12">
+      <c r="N4" s="12">
         <v>624</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="P4" t="s">
         <v>251</v>
       </c>
-      <c r="R4">
+      <c r="Q4">
         <v>234958</v>
       </c>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:19">
       <c r="A5">
         <v>12</v>
       </c>
@@ -3656,28 +3730,25 @@
         <v>121</v>
       </c>
       <c r="K5">
-        <v>74626</v>
+        <v>77920</v>
       </c>
       <c r="L5">
-        <v>77920</v>
+        <v>78719</v>
       </c>
       <c r="M5">
-        <v>78719</v>
-      </c>
-      <c r="N5">
         <v>79289</v>
       </c>
-      <c r="O5" s="12">
+      <c r="N5" s="12">
         <v>79386</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="P5" t="s">
         <v>252</v>
       </c>
-      <c r="R5">
+      <c r="Q5">
         <v>367</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:19">
       <c r="A6">
         <v>21</v>
       </c>
@@ -3706,28 +3777,25 @@
         <v>5</v>
       </c>
       <c r="K6">
-        <v>22781</v>
+        <v>22208</v>
       </c>
       <c r="L6">
-        <v>22208</v>
+        <v>22086</v>
       </c>
       <c r="M6">
-        <v>22086</v>
-      </c>
-      <c r="N6">
         <v>21052</v>
       </c>
-      <c r="O6" s="12">
+      <c r="N6" s="12">
         <v>30453</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="P6" t="s">
         <v>253</v>
       </c>
-      <c r="R6">
+      <c r="Q6">
         <v>139</v>
       </c>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:19">
       <c r="A7">
         <v>23</v>
       </c>
@@ -3756,22 +3824,19 @@
         <v>128</v>
       </c>
       <c r="K7">
-        <v>352835</v>
+        <v>328019</v>
       </c>
       <c r="L7">
-        <v>328019</v>
+        <v>307048</v>
       </c>
       <c r="M7">
-        <v>307048</v>
-      </c>
-      <c r="N7">
         <v>335079</v>
       </c>
-      <c r="O7" s="12">
+      <c r="N7" s="12">
         <v>5827</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:19">
       <c r="A8">
         <v>24</v>
       </c>
@@ -3800,25 +3865,22 @@
         <v>6</v>
       </c>
       <c r="K8">
-        <v>8873</v>
+        <v>16065</v>
       </c>
       <c r="L8">
-        <v>16065</v>
+        <v>24513</v>
       </c>
       <c r="M8">
-        <v>24513</v>
-      </c>
-      <c r="N8">
         <v>20221</v>
       </c>
-      <c r="O8" s="12">
+      <c r="N8" s="12">
         <v>33420</v>
       </c>
-      <c r="Q8" s="1" t="s">
+      <c r="P8" s="1" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:19">
       <c r="A9">
         <v>26</v>
       </c>
@@ -3847,28 +3909,25 @@
         <v>274</v>
       </c>
       <c r="K9">
-        <v>125130</v>
+        <v>131883</v>
       </c>
       <c r="L9">
-        <v>131883</v>
+        <v>141117</v>
       </c>
       <c r="M9">
-        <v>141117</v>
-      </c>
-      <c r="N9">
         <v>170589</v>
       </c>
-      <c r="O9" s="12">
+      <c r="N9" s="12">
         <v>95314</v>
       </c>
-      <c r="Q9" s="8" t="s">
+      <c r="P9" s="8" t="s">
         <v>255</v>
       </c>
-      <c r="R9">
+      <c r="Q9">
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:19">
       <c r="A10">
         <v>27</v>
       </c>
@@ -3897,28 +3956,25 @@
         <v>275</v>
       </c>
       <c r="K10">
-        <v>3561</v>
+        <v>901</v>
       </c>
       <c r="L10">
-        <v>901</v>
+        <v>1316</v>
       </c>
       <c r="M10">
-        <v>1316</v>
-      </c>
-      <c r="N10">
         <v>1212</v>
       </c>
-      <c r="O10" s="12">
+      <c r="N10" s="12">
         <v>2059</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="P10" t="s">
         <v>256</v>
       </c>
-      <c r="R10">
+      <c r="Q10">
         <v>152</v>
       </c>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:19">
       <c r="A11">
         <v>28</v>
       </c>
@@ -3947,28 +4003,25 @@
         <v>4</v>
       </c>
       <c r="K11">
-        <v>6050</v>
+        <v>6779</v>
       </c>
       <c r="L11">
-        <v>6779</v>
+        <v>6903</v>
       </c>
       <c r="M11">
-        <v>6903</v>
-      </c>
-      <c r="N11">
         <v>5930</v>
       </c>
-      <c r="O11" s="12">
+      <c r="N11" s="12">
         <v>5591</v>
       </c>
-      <c r="Q11" t="s">
+      <c r="P11" t="s">
         <v>257</v>
       </c>
-      <c r="R11">
+      <c r="Q11">
         <v>134</v>
       </c>
     </row>
-    <row r="12" spans="1:20">
+    <row r="12" spans="1:19">
       <c r="A12">
         <v>36</v>
       </c>
@@ -3996,17 +4049,17 @@
       <c r="J12" t="s">
         <v>291</v>
       </c>
-      <c r="O12" s="12">
+      <c r="N12" s="12">
         <v>358045</v>
       </c>
-      <c r="Q12" t="s">
+      <c r="P12" t="s">
         <v>258</v>
       </c>
-      <c r="R12">
+      <c r="Q12">
         <v>113</v>
       </c>
     </row>
-    <row r="13" spans="1:20">
+    <row r="13" spans="1:19">
       <c r="A13">
         <v>37</v>
       </c>
@@ -4032,19 +4085,19 @@
         <v>11</v>
       </c>
       <c r="J13" t="s">
-        <v>298</v>
-      </c>
-      <c r="O13" s="12">
+        <v>294</v>
+      </c>
+      <c r="N13" s="12">
         <v>287484</v>
       </c>
-      <c r="Q13" t="s">
+      <c r="P13" t="s">
         <v>259</v>
       </c>
-      <c r="R13">
+      <c r="Q13">
         <v>95</v>
       </c>
     </row>
-    <row r="14" spans="1:20">
+    <row r="14" spans="1:19">
       <c r="A14">
         <v>38</v>
       </c>
@@ -4070,19 +4123,19 @@
         <v>12</v>
       </c>
       <c r="J14" t="s">
-        <v>299</v>
-      </c>
-      <c r="O14" s="12">
+        <v>295</v>
+      </c>
+      <c r="N14" s="12">
         <v>16624</v>
       </c>
-      <c r="Q14" t="s">
+      <c r="P14" t="s">
         <v>260</v>
       </c>
-      <c r="R14">
+      <c r="Q14">
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:20">
+    <row r="15" spans="1:19">
       <c r="A15">
         <v>43</v>
       </c>
@@ -4108,13 +4161,13 @@
         <v>13</v>
       </c>
       <c r="J15" t="s">
-        <v>300</v>
-      </c>
-      <c r="O15" s="12">
+        <v>296</v>
+      </c>
+      <c r="N15" s="12">
         <v>12699</v>
       </c>
     </row>
-    <row r="16" spans="1:20">
+    <row r="16" spans="1:19">
       <c r="A16">
         <v>44</v>
       </c>
@@ -4140,16 +4193,16 @@
         <v>14</v>
       </c>
       <c r="J16" t="s">
-        <v>301</v>
-      </c>
-      <c r="O16" s="12">
+        <v>297</v>
+      </c>
+      <c r="N16" s="12">
         <v>15658</v>
       </c>
-      <c r="Q16" s="1" t="s">
+      <c r="P16" s="1" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="17" spans="1:25">
+    <row r="17" spans="1:24">
       <c r="A17">
         <v>47</v>
       </c>
@@ -4175,19 +4228,19 @@
         <v>15</v>
       </c>
       <c r="J17" t="s">
-        <v>302</v>
-      </c>
-      <c r="O17" s="12">
+        <v>298</v>
+      </c>
+      <c r="N17" s="12">
         <v>1134</v>
       </c>
-      <c r="Q17" t="s">
+      <c r="P17" t="s">
         <v>250</v>
       </c>
-      <c r="R17">
+      <c r="Q17">
         <v>592</v>
       </c>
     </row>
-    <row r="18" spans="1:25">
+    <row r="18" spans="1:24">
       <c r="A18">
         <v>53</v>
       </c>
@@ -4215,17 +4268,17 @@
       <c r="J18" t="s">
         <v>292</v>
       </c>
-      <c r="O18" s="12">
+      <c r="N18" s="12">
         <v>21740</v>
       </c>
-      <c r="Q18" t="s">
+      <c r="P18" t="s">
         <v>262</v>
       </c>
-      <c r="R18">
+      <c r="Q18">
         <v>218403</v>
       </c>
     </row>
-    <row r="19" spans="1:25">
+    <row r="19" spans="1:24">
       <c r="A19">
         <v>58</v>
       </c>
@@ -4252,19 +4305,19 @@
         <v>17</v>
       </c>
       <c r="J19" t="s">
-        <v>297</v>
-      </c>
-      <c r="O19" s="12">
+        <v>293</v>
+      </c>
+      <c r="N19" s="12">
         <v>12590</v>
       </c>
-      <c r="Q19" t="s">
+      <c r="P19" t="s">
         <v>263</v>
       </c>
-      <c r="R19">
+      <c r="Q19">
         <v>439</v>
       </c>
     </row>
-    <row r="20" spans="1:25">
+    <row r="20" spans="1:24">
       <c r="A20">
         <v>59</v>
       </c>
@@ -4290,16 +4343,15 @@
       <c r="I20" s="3"/>
       <c r="J20" s="9"/>
       <c r="K20" s="9"/>
-      <c r="L20" s="9"/>
-      <c r="O20" s="12"/>
-      <c r="Q20" t="s">
+      <c r="N20" s="12"/>
+      <c r="P20" t="s">
         <v>264</v>
       </c>
-      <c r="R20">
+      <c r="Q20">
         <v>208212</v>
       </c>
     </row>
-    <row r="21" spans="1:25">
+    <row r="21" spans="1:24">
       <c r="A21">
         <v>61</v>
       </c>
@@ -4325,10 +4377,9 @@
       <c r="I21" s="3"/>
       <c r="J21" s="9"/>
       <c r="K21" s="9"/>
-      <c r="L21" s="9"/>
-      <c r="O21" s="12"/>
-    </row>
-    <row r="22" spans="1:25">
+      <c r="N21" s="12"/>
+    </row>
+    <row r="22" spans="1:24">
       <c r="A22">
         <v>63</v>
       </c>
@@ -4354,31 +4405,30 @@
       <c r="I22" s="3"/>
       <c r="J22" s="9"/>
       <c r="K22" s="9"/>
-      <c r="L22" s="9"/>
-      <c r="O22" s="12"/>
+      <c r="N22" s="12"/>
+      <c r="R22" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="S22" s="1" t="s">
-        <v>0</v>
+        <v>267</v>
       </c>
       <c r="T22" s="1" t="s">
-        <v>267</v>
+        <v>79</v>
       </c>
       <c r="U22" s="1" t="s">
-        <v>79</v>
+        <v>128</v>
       </c>
       <c r="V22" s="1" t="s">
-        <v>128</v>
+        <v>268</v>
       </c>
       <c r="W22" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="X22" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="Y22" s="1" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="23" spans="1:25">
+    <row r="23" spans="1:24">
       <c r="A23">
         <v>87</v>
       </c>
@@ -4401,36 +4451,42 @@
         <v>0</v>
       </c>
       <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="9"/>
-      <c r="O23" s="12"/>
-      <c r="Q23" s="1" t="s">
+      <c r="I23" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="J23" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="K23" t="s">
+        <v>300</v>
+      </c>
+      <c r="N23" s="12"/>
+      <c r="P23" s="1" t="s">
         <v>250</v>
       </c>
+      <c r="Q23">
+        <v>364</v>
+      </c>
       <c r="R23">
-        <v>364</v>
+        <v>28</v>
       </c>
       <c r="S23">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="T23">
-        <v>25</v>
+        <v>326</v>
       </c>
       <c r="U23">
-        <v>326</v>
+        <v>146</v>
       </c>
       <c r="V23">
-        <v>146</v>
+        <v>5</v>
       </c>
       <c r="W23">
-        <v>5</v>
-      </c>
-      <c r="X23">
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:25">
+    <row r="24" spans="1:24">
       <c r="A24">
         <v>111</v>
       </c>
@@ -4453,37 +4509,42 @@
         <v>5930</v>
       </c>
       <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="9"/>
-      <c r="K24" s="9"/>
-      <c r="L24" s="9"/>
-      <c r="O24" s="12"/>
-      <c r="Q24" s="1" t="s">
+      <c r="I24" s="3">
+        <v>0</v>
+      </c>
+      <c r="J24" s="9" t="s">
+        <v>307</v>
+      </c>
+      <c r="K24" s="9">
+        <v>3961</v>
+      </c>
+      <c r="N24" s="12"/>
+      <c r="P24" s="1" t="s">
         <v>265</v>
       </c>
+      <c r="Q24">
+        <v>120899</v>
+      </c>
       <c r="R24">
-        <v>120899</v>
+        <v>879</v>
       </c>
       <c r="S24">
-        <v>879</v>
+        <v>327</v>
       </c>
       <c r="T24">
-        <v>327</v>
+        <v>83225</v>
       </c>
       <c r="U24">
-        <v>83225</v>
+        <v>2662</v>
       </c>
       <c r="V24">
-        <v>2662</v>
+        <v>162</v>
       </c>
       <c r="W24">
-        <v>162</v>
-      </c>
-      <c r="X24">
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:25">
+    <row r="25" spans="1:24">
       <c r="A25">
         <v>121</v>
       </c>
@@ -4506,35 +4567,42 @@
         <v>69674</v>
       </c>
       <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="9"/>
-      <c r="O25" s="12"/>
-      <c r="Q25" s="1" t="s">
+      <c r="I25" s="3">
+        <v>20</v>
+      </c>
+      <c r="J25" s="9" t="s">
+        <v>306</v>
+      </c>
+      <c r="K25">
+        <v>150909</v>
+      </c>
+      <c r="N25" s="12"/>
+      <c r="P25" s="1" t="s">
         <v>266</v>
       </c>
+      <c r="Q25">
+        <v>16978056</v>
+      </c>
       <c r="R25">
-        <v>16978056</v>
+        <v>8135</v>
       </c>
       <c r="S25">
-        <v>8135</v>
+        <v>24644</v>
       </c>
       <c r="T25">
-        <v>24644</v>
+        <v>3791960</v>
       </c>
       <c r="U25">
-        <v>3791960</v>
+        <v>7131</v>
       </c>
       <c r="V25">
-        <v>7131</v>
-      </c>
-      <c r="W25">
-        <v>1</v>
-      </c>
-      <c r="X25" t="s">
+        <v>1</v>
+      </c>
+      <c r="W25" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="26" spans="1:25">
+    <row r="26" spans="1:24">
       <c r="A26">
         <v>122</v>
       </c>
@@ -4558,12 +4626,17 @@
       </c>
       <c r="H26" s="3"/>
       <c r="I26" s="3">
-        <v>2012</v>
-      </c>
-      <c r="J26" s="9"/>
-      <c r="O26" s="12"/>
-    </row>
-    <row r="27" spans="1:25">
+        <v>40</v>
+      </c>
+      <c r="J26" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="K26">
+        <v>109345</v>
+      </c>
+      <c r="N26" s="12"/>
+    </row>
+    <row r="27" spans="1:24">
       <c r="A27">
         <v>123</v>
       </c>
@@ -4585,21 +4658,18 @@
       <c r="G27">
         <v>1255</v>
       </c>
-      <c r="I27" s="14">
-        <v>0</v>
-      </c>
-      <c r="J27" s="14" t="s">
-        <v>293</v>
-      </c>
-      <c r="K27" s="15">
-        <v>3961</v>
-      </c>
-      <c r="L27" s="11"/>
-      <c r="O27" s="12">
-        <v>116382</v>
-      </c>
-    </row>
-    <row r="28" spans="1:25">
+      <c r="I27" s="13">
+        <v>60</v>
+      </c>
+      <c r="J27" s="13" t="s">
+        <v>302</v>
+      </c>
+      <c r="K27" s="11" t="s">
+        <v>303</v>
+      </c>
+      <c r="N27" s="12"/>
+    </row>
+    <row r="28" spans="1:24">
       <c r="A28">
         <v>124</v>
       </c>
@@ -4621,21 +4691,18 @@
       <c r="G28">
         <v>467</v>
       </c>
-      <c r="I28" s="14">
-        <v>30</v>
-      </c>
-      <c r="J28" s="14" t="s">
-        <v>294</v>
-      </c>
-      <c r="K28" s="15">
-        <v>68981</v>
-      </c>
-      <c r="L28" s="11"/>
-      <c r="O28" s="12">
-        <v>109113</v>
-      </c>
-    </row>
-    <row r="29" spans="1:25">
+      <c r="I28" s="13">
+        <v>80</v>
+      </c>
+      <c r="J28" s="13" t="s">
+        <v>304</v>
+      </c>
+      <c r="K28" s="11" t="s">
+        <v>305</v>
+      </c>
+      <c r="N28" s="12"/>
+    </row>
+    <row r="29" spans="1:24">
       <c r="A29">
         <v>131</v>
       </c>
@@ -4657,20 +4724,11 @@
       <c r="G29">
         <v>1212</v>
       </c>
-      <c r="I29" s="14">
-        <v>60</v>
-      </c>
-      <c r="J29" s="14" t="s">
-        <v>291</v>
-      </c>
-      <c r="K29" s="15">
-        <v>1273</v>
-      </c>
-      <c r="O29" s="12">
-        <v>393992</v>
-      </c>
-    </row>
-    <row r="30" spans="1:25">
+      <c r="I29" s="13"/>
+      <c r="J29" s="13"/>
+      <c r="N29" s="12"/>
+    </row>
+    <row r="30" spans="1:24">
       <c r="A30">
         <v>141</v>
       </c>
@@ -4692,21 +4750,12 @@
       <c r="G30">
         <v>21032</v>
       </c>
-      <c r="I30" s="14">
-        <v>90</v>
-      </c>
-      <c r="J30" s="14" t="s">
-        <v>296</v>
-      </c>
-      <c r="K30" s="15">
-        <v>82527</v>
-      </c>
-      <c r="L30" s="3"/>
-      <c r="O30" s="12">
-        <v>313793</v>
-      </c>
-    </row>
-    <row r="31" spans="1:25">
+      <c r="I30" s="13"/>
+      <c r="J30" s="13"/>
+      <c r="K30" s="3"/>
+      <c r="N30" s="12"/>
+    </row>
+    <row r="31" spans="1:24">
       <c r="A31">
         <v>142</v>
       </c>
@@ -4728,20 +4777,11 @@
       <c r="G31">
         <v>18</v>
       </c>
-      <c r="I31" s="14">
-        <v>120</v>
-      </c>
-      <c r="J31" s="14" t="s">
-        <v>295</v>
-      </c>
-      <c r="K31" s="15">
-        <v>21943</v>
-      </c>
-      <c r="O31" s="12">
-        <v>158674</v>
-      </c>
-    </row>
-    <row r="32" spans="1:25">
+      <c r="I31" s="13"/>
+      <c r="J31" s="13"/>
+      <c r="N31" s="12"/>
+    </row>
+    <row r="32" spans="1:24">
       <c r="A32">
         <v>143</v>
       </c>
@@ -4763,15 +4803,12 @@
       <c r="G32">
         <v>2</v>
       </c>
-      <c r="I32" s="14"/>
-      <c r="J32" s="14"/>
-      <c r="K32" s="15">
-        <v>3671</v>
-      </c>
-      <c r="L32" s="3"/>
-      <c r="O32" s="12"/>
-    </row>
-    <row r="33" spans="1:15">
+      <c r="I32" s="13"/>
+      <c r="J32" s="13"/>
+      <c r="K32" s="3"/>
+      <c r="N32" s="12"/>
+    </row>
+    <row r="33" spans="1:14">
       <c r="A33">
         <v>152</v>
       </c>
@@ -4793,15 +4830,12 @@
       <c r="G33">
         <v>0</v>
       </c>
-      <c r="I33" s="14"/>
-      <c r="J33" s="14"/>
-      <c r="K33" s="15">
-        <v>22498</v>
-      </c>
-      <c r="L33" s="3"/>
-      <c r="O33" s="12"/>
-    </row>
-    <row r="34" spans="1:15">
+      <c r="I33" s="13"/>
+      <c r="J33" s="13"/>
+      <c r="K33" s="3"/>
+      <c r="N33" s="12"/>
+    </row>
+    <row r="34" spans="1:14">
       <c r="A34">
         <v>176</v>
       </c>
@@ -4823,14 +4857,11 @@
       <c r="G34">
         <v>170589</v>
       </c>
-      <c r="I34" s="14"/>
-      <c r="J34" s="14"/>
-      <c r="K34" s="15">
-        <v>116881</v>
-      </c>
-      <c r="O34" s="12"/>
-    </row>
-    <row r="35" spans="1:15">
+      <c r="I34" s="13"/>
+      <c r="J34" s="13"/>
+      <c r="N34" s="12"/>
+    </row>
+    <row r="35" spans="1:14">
       <c r="A35">
         <v>190</v>
       </c>
@@ -4852,14 +4883,11 @@
       <c r="G35">
         <v>4921</v>
       </c>
-      <c r="I35" s="14"/>
-      <c r="J35" s="14"/>
-      <c r="K35" s="15">
-        <v>1639</v>
-      </c>
-      <c r="O35" s="12"/>
-    </row>
-    <row r="36" spans="1:15">
+      <c r="I35" s="13"/>
+      <c r="J35" s="13"/>
+      <c r="N35" s="12"/>
+    </row>
+    <row r="36" spans="1:14">
       <c r="A36">
         <v>195</v>
       </c>
@@ -4881,14 +4909,11 @@
       <c r="G36">
         <v>15300</v>
       </c>
-      <c r="I36" s="14"/>
-      <c r="J36" s="14"/>
-      <c r="K36" s="15">
-        <v>6312</v>
-      </c>
-      <c r="O36" s="12"/>
-    </row>
-    <row r="37" spans="1:15">
+      <c r="I36" s="13"/>
+      <c r="J36" s="13"/>
+      <c r="N36" s="12"/>
+    </row>
+    <row r="37" spans="1:14">
       <c r="A37">
         <v>241</v>
       </c>
@@ -4910,1735 +4935,1369 @@
       <c r="G37">
         <v>122</v>
       </c>
-      <c r="I37" s="14"/>
-      <c r="J37" s="14"/>
-      <c r="K37" s="15">
-        <v>220948</v>
-      </c>
-      <c r="O37" s="12"/>
-    </row>
-    <row r="38" spans="1:15">
-      <c r="I38" s="14"/>
-      <c r="J38" s="14"/>
-      <c r="K38" s="15">
-        <v>210174</v>
-      </c>
-      <c r="O38" s="12"/>
-    </row>
-    <row r="39" spans="1:15">
-      <c r="I39" s="14"/>
-      <c r="J39" s="14"/>
-      <c r="K39" s="15">
-        <v>32510</v>
-      </c>
-      <c r="O39" s="9"/>
-    </row>
-    <row r="40" spans="1:15">
-      <c r="I40" s="14"/>
-      <c r="J40" s="14"/>
-      <c r="K40" s="15">
-        <v>31584</v>
-      </c>
-      <c r="O40" s="12"/>
-    </row>
-    <row r="41" spans="1:15">
-      <c r="I41" s="14"/>
-      <c r="J41" s="14"/>
-      <c r="K41" s="15">
-        <v>78955</v>
-      </c>
-      <c r="O41" s="12"/>
-    </row>
-    <row r="42" spans="1:15">
+      <c r="I37" s="13"/>
+      <c r="J37" s="13"/>
+      <c r="N37" s="12"/>
+    </row>
+    <row r="38" spans="1:14">
+      <c r="I38" s="13"/>
+      <c r="J38" s="13"/>
+      <c r="N38" s="12"/>
+    </row>
+    <row r="39" spans="1:14">
+      <c r="I39" s="13"/>
+      <c r="J39" s="13"/>
+      <c r="N39" s="9"/>
+    </row>
+    <row r="40" spans="1:14">
+      <c r="I40" s="13"/>
+      <c r="J40" s="13"/>
+      <c r="N40" s="12"/>
+    </row>
+    <row r="41" spans="1:14">
+      <c r="I41" s="13"/>
+      <c r="J41" s="13"/>
+      <c r="N41" s="12"/>
+    </row>
+    <row r="42" spans="1:14">
       <c r="I42" s="3"/>
-      <c r="J42" s="14"/>
-      <c r="K42" s="15">
-        <v>48492</v>
-      </c>
-      <c r="O42" s="12"/>
-    </row>
-    <row r="43" spans="1:15">
-      <c r="I43" s="14"/>
-      <c r="J43" s="14"/>
-      <c r="K43" s="15">
-        <v>40132</v>
-      </c>
-      <c r="L43" s="10"/>
-      <c r="O43" s="12"/>
-    </row>
-    <row r="44" spans="1:15">
-      <c r="I44" s="14"/>
-      <c r="J44" s="14"/>
-      <c r="K44" s="15">
-        <v>5762</v>
-      </c>
-      <c r="O44" s="12"/>
-    </row>
-    <row r="45" spans="1:15">
+      <c r="J42" s="13"/>
+      <c r="N42" s="12"/>
+    </row>
+    <row r="43" spans="1:14">
+      <c r="I43" s="13"/>
+      <c r="J43" s="13"/>
+      <c r="K43" s="10"/>
+      <c r="N43" s="12"/>
+    </row>
+    <row r="44" spans="1:14">
+      <c r="I44" s="13"/>
+      <c r="J44" s="13"/>
+      <c r="N44" s="12"/>
+    </row>
+    <row r="45" spans="1:14">
       <c r="I45" s="3"/>
-      <c r="J45" s="16"/>
-      <c r="K45" s="15">
-        <v>52552</v>
-      </c>
-    </row>
-    <row r="46" spans="1:15">
+      <c r="J45" s="14"/>
+    </row>
+    <row r="46" spans="1:14">
       <c r="I46" s="3"/>
-      <c r="J46" s="16"/>
-      <c r="K46" s="15">
-        <v>7594</v>
-      </c>
-    </row>
-    <row r="47" spans="1:15">
+      <c r="J46" s="14"/>
+    </row>
+    <row r="47" spans="1:14">
       <c r="I47" s="3"/>
-      <c r="J47" s="16"/>
-      <c r="K47" s="15">
-        <v>4158</v>
-      </c>
-    </row>
-    <row r="48" spans="1:15">
+      <c r="J47" s="14"/>
+    </row>
+    <row r="48" spans="1:14">
       <c r="I48" s="3"/>
-      <c r="J48" s="16"/>
-      <c r="K48" s="15">
-        <v>7906</v>
-      </c>
-    </row>
-    <row r="49" spans="9:11">
+      <c r="J48" s="14"/>
+    </row>
+    <row r="49" spans="9:10">
       <c r="I49" s="3"/>
-      <c r="J49" s="16"/>
-      <c r="K49" s="15">
-        <v>7150</v>
-      </c>
-    </row>
-    <row r="50" spans="9:11">
+      <c r="J49" s="14"/>
+    </row>
+    <row r="50" spans="9:10">
       <c r="I50" s="3"/>
-      <c r="J50" s="16"/>
-      <c r="K50" s="15">
-        <v>14351</v>
-      </c>
-    </row>
-    <row r="51" spans="9:11">
+      <c r="J50" s="14"/>
+    </row>
+    <row r="51" spans="9:10">
       <c r="I51" s="3"/>
       <c r="J51" s="10"/>
-      <c r="K51" s="10"/>
-    </row>
-    <row r="52" spans="9:11">
+    </row>
+    <row r="52" spans="9:10">
       <c r="I52" s="3"/>
       <c r="J52" s="10"/>
-      <c r="K52" s="10"/>
-    </row>
-    <row r="53" spans="9:11">
+    </row>
+    <row r="53" spans="9:10">
       <c r="I53" s="3"/>
       <c r="J53" s="10"/>
-      <c r="K53" s="10"/>
-    </row>
-    <row r="54" spans="9:11">
+    </row>
+    <row r="54" spans="9:10">
       <c r="I54" s="3"/>
       <c r="J54" s="10"/>
-      <c r="K54" s="10"/>
-    </row>
-    <row r="55" spans="9:11">
+    </row>
+    <row r="55" spans="9:10">
       <c r="I55" s="3"/>
       <c r="J55" s="10"/>
-      <c r="K55" s="10"/>
-    </row>
-    <row r="56" spans="9:11">
+    </row>
+    <row r="56" spans="9:10">
       <c r="I56" s="3"/>
       <c r="J56" s="10"/>
-      <c r="K56" s="10"/>
-    </row>
-    <row r="57" spans="9:11">
+    </row>
+    <row r="57" spans="9:10">
       <c r="I57" s="3"/>
       <c r="J57" s="10"/>
-      <c r="K57" s="10"/>
-    </row>
-    <row r="58" spans="9:11">
+    </row>
+    <row r="58" spans="9:10">
       <c r="I58" s="3"/>
       <c r="J58" s="10"/>
-      <c r="K58" s="10"/>
-    </row>
-    <row r="59" spans="9:11">
+    </row>
+    <row r="59" spans="9:10">
       <c r="I59" s="3"/>
       <c r="J59" s="10"/>
-      <c r="K59" s="10"/>
-    </row>
-    <row r="60" spans="9:11">
+    </row>
+    <row r="60" spans="9:10">
       <c r="I60" s="3"/>
       <c r="J60" s="10"/>
-      <c r="K60" s="10"/>
-    </row>
-    <row r="61" spans="9:11">
+    </row>
+    <row r="61" spans="9:10">
       <c r="I61" s="3"/>
       <c r="J61" s="10"/>
-      <c r="K61" s="10"/>
-    </row>
-    <row r="62" spans="9:11">
+    </row>
+    <row r="62" spans="9:10">
       <c r="I62" s="3"/>
       <c r="J62" s="10"/>
-      <c r="K62" s="10"/>
-    </row>
-    <row r="63" spans="9:11">
+    </row>
+    <row r="63" spans="9:10">
       <c r="I63" s="3"/>
       <c r="J63" s="10"/>
-      <c r="K63" s="10"/>
-    </row>
-    <row r="64" spans="9:11">
+    </row>
+    <row r="64" spans="9:10">
       <c r="I64" s="3"/>
       <c r="J64" s="10"/>
-      <c r="K64" s="10"/>
-    </row>
-    <row r="65" spans="9:11">
+    </row>
+    <row r="65" spans="9:10">
       <c r="I65" s="3"/>
       <c r="J65" s="10"/>
-      <c r="K65" s="10"/>
-    </row>
-    <row r="66" spans="9:11">
+    </row>
+    <row r="66" spans="9:10">
       <c r="I66" s="3"/>
       <c r="J66" s="10"/>
-      <c r="K66" s="10"/>
-    </row>
-    <row r="67" spans="9:11">
+    </row>
+    <row r="67" spans="9:10">
       <c r="I67" s="3"/>
       <c r="J67" s="10"/>
-      <c r="K67" s="10"/>
-    </row>
-    <row r="68" spans="9:11">
+    </row>
+    <row r="68" spans="9:10">
       <c r="I68" s="3"/>
       <c r="J68" s="10"/>
-      <c r="K68" s="10"/>
-    </row>
-    <row r="69" spans="9:11">
+    </row>
+    <row r="69" spans="9:10">
       <c r="I69" s="3"/>
       <c r="J69" s="10"/>
-      <c r="K69" s="10"/>
-    </row>
-    <row r="70" spans="9:11">
+    </row>
+    <row r="70" spans="9:10">
       <c r="I70" s="3"/>
       <c r="J70" s="10"/>
-      <c r="K70" s="10"/>
-    </row>
-    <row r="71" spans="9:11">
+    </row>
+    <row r="71" spans="9:10">
       <c r="I71" s="3"/>
       <c r="J71" s="10"/>
-      <c r="K71" s="10"/>
-    </row>
-    <row r="72" spans="9:11">
+    </row>
+    <row r="72" spans="9:10">
       <c r="I72" s="3"/>
       <c r="J72" s="10"/>
-      <c r="K72" s="10"/>
-    </row>
-    <row r="73" spans="9:11">
+    </row>
+    <row r="73" spans="9:10">
       <c r="I73" s="3"/>
       <c r="J73" s="10"/>
-      <c r="K73" s="10"/>
-    </row>
-    <row r="74" spans="9:11">
+    </row>
+    <row r="74" spans="9:10">
       <c r="I74" s="3"/>
       <c r="J74" s="10"/>
-      <c r="K74" s="10"/>
-    </row>
-    <row r="75" spans="9:11">
+    </row>
+    <row r="75" spans="9:10">
       <c r="I75" s="3"/>
       <c r="J75" s="10"/>
-      <c r="K75" s="10"/>
-    </row>
-    <row r="76" spans="9:11">
+    </row>
+    <row r="76" spans="9:10">
       <c r="I76" s="3"/>
       <c r="J76" s="10"/>
-      <c r="K76" s="10"/>
-    </row>
-    <row r="77" spans="9:11">
+    </row>
+    <row r="77" spans="9:10">
       <c r="I77" s="3"/>
       <c r="J77" s="10"/>
-      <c r="K77" s="10"/>
-    </row>
-    <row r="78" spans="9:11">
+    </row>
+    <row r="78" spans="9:10">
       <c r="I78" s="3"/>
       <c r="J78" s="10"/>
-      <c r="K78" s="10"/>
-    </row>
-    <row r="79" spans="9:11">
+    </row>
+    <row r="79" spans="9:10">
       <c r="I79" s="3"/>
       <c r="J79" s="10"/>
-      <c r="K79" s="10"/>
-    </row>
-    <row r="80" spans="9:11">
+    </row>
+    <row r="80" spans="9:10">
       <c r="I80" s="3"/>
       <c r="J80" s="10"/>
-      <c r="K80" s="10"/>
-    </row>
-    <row r="81" spans="9:11">
+    </row>
+    <row r="81" spans="9:10">
       <c r="I81" s="3"/>
       <c r="J81" s="10"/>
-      <c r="K81" s="10"/>
-    </row>
-    <row r="82" spans="9:11">
+    </row>
+    <row r="82" spans="9:10">
       <c r="I82" s="3"/>
       <c r="J82" s="10"/>
-      <c r="K82" s="10"/>
-    </row>
-    <row r="83" spans="9:11">
+    </row>
+    <row r="83" spans="9:10">
       <c r="I83" s="3"/>
       <c r="J83" s="10"/>
-      <c r="K83" s="10"/>
-    </row>
-    <row r="84" spans="9:11">
+    </row>
+    <row r="84" spans="9:10">
       <c r="I84" s="3"/>
       <c r="J84" s="10"/>
-      <c r="K84" s="10"/>
-    </row>
-    <row r="85" spans="9:11">
+    </row>
+    <row r="85" spans="9:10">
       <c r="I85" s="3"/>
       <c r="J85" s="10"/>
-      <c r="K85" s="10"/>
-    </row>
-    <row r="86" spans="9:11">
+    </row>
+    <row r="86" spans="9:10">
       <c r="I86" s="3"/>
       <c r="J86" s="10"/>
-      <c r="K86" s="10"/>
-    </row>
-    <row r="87" spans="9:11">
+    </row>
+    <row r="87" spans="9:10">
       <c r="I87" s="3"/>
       <c r="J87" s="10"/>
-      <c r="K87" s="10"/>
-    </row>
-    <row r="88" spans="9:11">
+    </row>
+    <row r="88" spans="9:10">
       <c r="I88" s="3"/>
       <c r="J88" s="10"/>
-      <c r="K88" s="10"/>
-    </row>
-    <row r="89" spans="9:11">
+    </row>
+    <row r="89" spans="9:10">
       <c r="I89" s="3"/>
       <c r="J89" s="10"/>
-      <c r="K89" s="10"/>
-    </row>
-    <row r="90" spans="9:11">
+    </row>
+    <row r="90" spans="9:10">
       <c r="I90" s="3"/>
       <c r="J90" s="10"/>
-      <c r="K90" s="10"/>
-    </row>
-    <row r="91" spans="9:11">
+    </row>
+    <row r="91" spans="9:10">
       <c r="I91" s="3"/>
       <c r="J91" s="10"/>
-      <c r="K91" s="10"/>
-    </row>
-    <row r="92" spans="9:11">
+    </row>
+    <row r="92" spans="9:10">
       <c r="I92" s="3"/>
       <c r="J92" s="10"/>
-      <c r="K92" s="10"/>
-    </row>
-    <row r="93" spans="9:11">
+    </row>
+    <row r="93" spans="9:10">
       <c r="I93" s="3"/>
       <c r="J93" s="10"/>
-      <c r="K93" s="10"/>
-    </row>
-    <row r="94" spans="9:11">
+    </row>
+    <row r="94" spans="9:10">
       <c r="I94" s="3"/>
       <c r="J94" s="10"/>
-      <c r="K94" s="10"/>
-    </row>
-    <row r="95" spans="9:11">
+    </row>
+    <row r="95" spans="9:10">
       <c r="I95" s="3"/>
       <c r="J95" s="10"/>
-      <c r="K95" s="10"/>
-    </row>
-    <row r="96" spans="9:11">
+    </row>
+    <row r="96" spans="9:10">
       <c r="I96" s="3"/>
       <c r="J96" s="10"/>
-      <c r="K96" s="10"/>
-    </row>
-    <row r="97" spans="9:11">
+    </row>
+    <row r="97" spans="9:10">
       <c r="I97" s="3"/>
       <c r="J97" s="10"/>
-      <c r="K97" s="10"/>
-    </row>
-    <row r="98" spans="9:11">
+    </row>
+    <row r="98" spans="9:10">
       <c r="I98" s="3"/>
       <c r="J98" s="10"/>
-      <c r="K98" s="10"/>
-    </row>
-    <row r="99" spans="9:11">
+    </row>
+    <row r="99" spans="9:10">
       <c r="I99" s="3"/>
       <c r="J99" s="10"/>
-      <c r="K99" s="10"/>
-    </row>
-    <row r="100" spans="9:11">
+    </row>
+    <row r="100" spans="9:10">
       <c r="I100" s="3"/>
       <c r="J100" s="10"/>
-      <c r="K100" s="10"/>
-    </row>
-    <row r="101" spans="9:11">
+    </row>
+    <row r="101" spans="9:10">
       <c r="I101" s="3"/>
       <c r="J101" s="10"/>
-      <c r="K101" s="10"/>
-    </row>
-    <row r="102" spans="9:11">
+    </row>
+    <row r="102" spans="9:10">
       <c r="I102" s="3"/>
       <c r="J102" s="10"/>
-      <c r="K102" s="10"/>
-    </row>
-    <row r="103" spans="9:11">
+    </row>
+    <row r="103" spans="9:10">
       <c r="I103" s="3"/>
       <c r="J103" s="10"/>
-      <c r="K103" s="10"/>
-    </row>
-    <row r="104" spans="9:11">
+    </row>
+    <row r="104" spans="9:10">
       <c r="I104" s="3"/>
       <c r="J104" s="10"/>
-      <c r="K104" s="10"/>
-    </row>
-    <row r="105" spans="9:11">
+    </row>
+    <row r="105" spans="9:10">
       <c r="I105" s="3"/>
       <c r="J105" s="10"/>
-      <c r="K105" s="10"/>
-    </row>
-    <row r="106" spans="9:11">
+    </row>
+    <row r="106" spans="9:10">
       <c r="I106" s="3"/>
       <c r="J106" s="10"/>
-      <c r="K106" s="10"/>
-    </row>
-    <row r="107" spans="9:11">
+    </row>
+    <row r="107" spans="9:10">
       <c r="I107" s="3"/>
       <c r="J107" s="10"/>
-      <c r="K107" s="10"/>
-    </row>
-    <row r="108" spans="9:11">
+    </row>
+    <row r="108" spans="9:10">
       <c r="I108" s="3"/>
       <c r="J108" s="10"/>
-      <c r="K108" s="10"/>
-    </row>
-    <row r="109" spans="9:11">
+    </row>
+    <row r="109" spans="9:10">
       <c r="I109" s="3"/>
       <c r="J109" s="10"/>
-      <c r="K109" s="10"/>
-    </row>
-    <row r="110" spans="9:11">
+    </row>
+    <row r="110" spans="9:10">
       <c r="I110" s="3"/>
       <c r="J110" s="10"/>
-      <c r="K110" s="10"/>
-    </row>
-    <row r="111" spans="9:11">
+    </row>
+    <row r="111" spans="9:10">
       <c r="I111" s="3"/>
       <c r="J111" s="10"/>
-      <c r="K111" s="10"/>
-    </row>
-    <row r="112" spans="9:11">
+    </row>
+    <row r="112" spans="9:10">
       <c r="I112" s="3"/>
       <c r="J112" s="10"/>
-      <c r="K112" s="10"/>
-    </row>
-    <row r="113" spans="9:11">
+    </row>
+    <row r="113" spans="9:10">
       <c r="I113" s="3"/>
       <c r="J113" s="10"/>
-      <c r="K113" s="10"/>
-    </row>
-    <row r="114" spans="9:11">
+    </row>
+    <row r="114" spans="9:10">
       <c r="I114" s="3"/>
       <c r="J114" s="10"/>
-      <c r="K114" s="10"/>
-    </row>
-    <row r="115" spans="9:11">
+    </row>
+    <row r="115" spans="9:10">
       <c r="I115" s="3"/>
       <c r="J115" s="10"/>
-      <c r="K115" s="10"/>
-    </row>
-    <row r="116" spans="9:11">
+    </row>
+    <row r="116" spans="9:10">
       <c r="I116" s="3"/>
       <c r="J116" s="10"/>
-      <c r="K116" s="10"/>
-    </row>
-    <row r="117" spans="9:11">
+    </row>
+    <row r="117" spans="9:10">
       <c r="I117" s="3"/>
       <c r="J117" s="10"/>
-      <c r="K117" s="10"/>
-    </row>
-    <row r="118" spans="9:11">
+    </row>
+    <row r="118" spans="9:10">
       <c r="I118" s="3"/>
       <c r="J118" s="10"/>
-      <c r="K118" s="10"/>
-    </row>
-    <row r="119" spans="9:11">
+    </row>
+    <row r="119" spans="9:10">
       <c r="I119" s="3"/>
       <c r="J119" s="10"/>
-      <c r="K119" s="10"/>
-    </row>
-    <row r="120" spans="9:11">
+    </row>
+    <row r="120" spans="9:10">
       <c r="I120" s="3"/>
       <c r="J120" s="10"/>
-      <c r="K120" s="10"/>
-    </row>
-    <row r="121" spans="9:11">
+    </row>
+    <row r="121" spans="9:10">
       <c r="I121" s="3"/>
       <c r="J121" s="10"/>
-      <c r="K121" s="10"/>
-    </row>
-    <row r="122" spans="9:11">
+    </row>
+    <row r="122" spans="9:10">
       <c r="I122" s="3"/>
       <c r="J122" s="10"/>
-      <c r="K122" s="10"/>
-    </row>
-    <row r="123" spans="9:11">
+    </row>
+    <row r="123" spans="9:10">
       <c r="I123" s="3"/>
       <c r="J123" s="10"/>
-      <c r="K123" s="10"/>
-    </row>
-    <row r="124" spans="9:11">
+    </row>
+    <row r="124" spans="9:10">
       <c r="I124" s="3"/>
       <c r="J124" s="10"/>
-      <c r="K124" s="10"/>
-    </row>
-    <row r="125" spans="9:11">
+    </row>
+    <row r="125" spans="9:10">
       <c r="I125" s="3"/>
       <c r="J125" s="10"/>
-      <c r="K125" s="10"/>
-    </row>
-    <row r="126" spans="9:11">
+    </row>
+    <row r="126" spans="9:10">
       <c r="I126" s="3"/>
       <c r="J126" s="10"/>
-      <c r="K126" s="10"/>
-    </row>
-    <row r="127" spans="9:11">
+    </row>
+    <row r="127" spans="9:10">
       <c r="I127" s="3"/>
       <c r="J127" s="10"/>
-      <c r="K127" s="10"/>
-    </row>
-    <row r="128" spans="9:11">
+    </row>
+    <row r="128" spans="9:10">
       <c r="I128" s="3"/>
       <c r="J128" s="10"/>
-      <c r="K128" s="10"/>
-    </row>
-    <row r="129" spans="9:11">
+    </row>
+    <row r="129" spans="9:10">
       <c r="I129" s="3"/>
       <c r="J129" s="10"/>
-      <c r="K129" s="10"/>
-    </row>
-    <row r="130" spans="9:11">
+    </row>
+    <row r="130" spans="9:10">
       <c r="I130" s="3"/>
       <c r="J130" s="10"/>
-      <c r="K130" s="10"/>
-    </row>
-    <row r="131" spans="9:11">
+    </row>
+    <row r="131" spans="9:10">
       <c r="I131" s="3"/>
       <c r="J131" s="10"/>
-      <c r="K131" s="10"/>
-    </row>
-    <row r="132" spans="9:11">
+    </row>
+    <row r="132" spans="9:10">
       <c r="I132" s="3"/>
       <c r="J132" s="10"/>
-      <c r="K132" s="10"/>
-    </row>
-    <row r="133" spans="9:11">
+    </row>
+    <row r="133" spans="9:10">
       <c r="I133" s="3"/>
       <c r="J133" s="10"/>
-      <c r="K133" s="10"/>
-    </row>
-    <row r="134" spans="9:11">
+    </row>
+    <row r="134" spans="9:10">
       <c r="I134" s="3"/>
       <c r="J134" s="10"/>
-      <c r="K134" s="10"/>
-    </row>
-    <row r="135" spans="9:11">
+    </row>
+    <row r="135" spans="9:10">
       <c r="I135" s="3"/>
       <c r="J135" s="10"/>
-      <c r="K135" s="10"/>
-    </row>
-    <row r="136" spans="9:11">
+    </row>
+    <row r="136" spans="9:10">
       <c r="I136" s="3"/>
       <c r="J136" s="10"/>
-      <c r="K136" s="10"/>
-    </row>
-    <row r="137" spans="9:11">
+    </row>
+    <row r="137" spans="9:10">
       <c r="I137" s="3"/>
       <c r="J137" s="10"/>
-      <c r="K137" s="10"/>
-    </row>
-    <row r="138" spans="9:11">
+    </row>
+    <row r="138" spans="9:10">
       <c r="I138" s="3"/>
       <c r="J138" s="10"/>
-      <c r="K138" s="10"/>
-    </row>
-    <row r="139" spans="9:11">
+    </row>
+    <row r="139" spans="9:10">
       <c r="I139" s="3"/>
       <c r="J139" s="10"/>
-      <c r="K139" s="10"/>
-    </row>
-    <row r="140" spans="9:11">
+    </row>
+    <row r="140" spans="9:10">
       <c r="I140" s="3"/>
       <c r="J140" s="10"/>
-      <c r="K140" s="10"/>
-    </row>
-    <row r="141" spans="9:11">
+    </row>
+    <row r="141" spans="9:10">
       <c r="I141" s="3"/>
       <c r="J141" s="10"/>
-      <c r="K141" s="10"/>
-    </row>
-    <row r="142" spans="9:11">
+    </row>
+    <row r="142" spans="9:10">
       <c r="I142" s="3"/>
       <c r="J142" s="10"/>
-      <c r="K142" s="10"/>
-    </row>
-    <row r="143" spans="9:11">
+    </row>
+    <row r="143" spans="9:10">
       <c r="I143" s="3"/>
       <c r="J143" s="10"/>
-      <c r="K143" s="10"/>
-    </row>
-    <row r="144" spans="9:11">
+    </row>
+    <row r="144" spans="9:10">
       <c r="I144" s="3"/>
       <c r="J144" s="10"/>
-      <c r="K144" s="10"/>
-    </row>
-    <row r="145" spans="9:11">
+    </row>
+    <row r="145" spans="9:10">
       <c r="I145" s="3"/>
       <c r="J145" s="10"/>
-      <c r="K145" s="10"/>
-    </row>
-    <row r="146" spans="9:11">
+    </row>
+    <row r="146" spans="9:10">
       <c r="I146" s="3"/>
       <c r="J146" s="10"/>
-      <c r="K146" s="10"/>
-    </row>
-    <row r="147" spans="9:11">
+    </row>
+    <row r="147" spans="9:10">
       <c r="I147" s="3"/>
       <c r="J147" s="10"/>
-      <c r="K147" s="10"/>
-    </row>
-    <row r="148" spans="9:11">
+    </row>
+    <row r="148" spans="9:10">
       <c r="I148" s="3"/>
       <c r="J148" s="10"/>
-      <c r="K148" s="10"/>
-    </row>
-    <row r="149" spans="9:11">
+    </row>
+    <row r="149" spans="9:10">
       <c r="I149" s="3"/>
       <c r="J149" s="10"/>
-      <c r="K149" s="10"/>
-    </row>
-    <row r="150" spans="9:11">
+    </row>
+    <row r="150" spans="9:10">
       <c r="I150" s="3"/>
       <c r="J150" s="10"/>
-      <c r="K150" s="10"/>
-    </row>
-    <row r="151" spans="9:11">
+    </row>
+    <row r="151" spans="9:10">
       <c r="I151" s="3"/>
       <c r="J151" s="10"/>
-      <c r="K151" s="10"/>
-    </row>
-    <row r="152" spans="9:11">
+    </row>
+    <row r="152" spans="9:10">
       <c r="I152" s="3"/>
       <c r="J152" s="10"/>
-      <c r="K152" s="10"/>
-    </row>
-    <row r="153" spans="9:11">
+    </row>
+    <row r="153" spans="9:10">
       <c r="I153" s="3"/>
       <c r="J153" s="10"/>
-      <c r="K153" s="10"/>
-    </row>
-    <row r="154" spans="9:11">
+    </row>
+    <row r="154" spans="9:10">
       <c r="I154" s="3"/>
       <c r="J154" s="10"/>
-      <c r="K154" s="10"/>
-    </row>
-    <row r="155" spans="9:11">
+    </row>
+    <row r="155" spans="9:10">
       <c r="I155" s="3"/>
       <c r="J155" s="10"/>
-      <c r="K155" s="10"/>
-    </row>
-    <row r="156" spans="9:11">
+    </row>
+    <row r="156" spans="9:10">
       <c r="I156" s="3"/>
       <c r="J156" s="10"/>
-      <c r="K156" s="10"/>
-    </row>
-    <row r="157" spans="9:11">
+    </row>
+    <row r="157" spans="9:10">
       <c r="I157" s="3"/>
       <c r="J157" s="10"/>
-      <c r="K157" s="10"/>
-    </row>
-    <row r="158" spans="9:11">
+    </row>
+    <row r="158" spans="9:10">
       <c r="I158" s="3"/>
       <c r="J158" s="10"/>
-      <c r="K158" s="10"/>
-    </row>
-    <row r="159" spans="9:11">
+    </row>
+    <row r="159" spans="9:10">
       <c r="I159" s="3"/>
       <c r="J159" s="10"/>
-      <c r="K159" s="10"/>
-    </row>
-    <row r="160" spans="9:11">
+    </row>
+    <row r="160" spans="9:10">
       <c r="I160" s="3"/>
       <c r="J160" s="10"/>
-      <c r="K160" s="10"/>
-    </row>
-    <row r="161" spans="9:11">
+    </row>
+    <row r="161" spans="9:10">
       <c r="I161" s="3"/>
       <c r="J161" s="10"/>
-      <c r="K161" s="10"/>
-    </row>
-    <row r="162" spans="9:11">
+    </row>
+    <row r="162" spans="9:10">
       <c r="I162" s="3"/>
       <c r="J162" s="10"/>
-      <c r="K162" s="10"/>
-    </row>
-    <row r="163" spans="9:11">
+    </row>
+    <row r="163" spans="9:10">
       <c r="I163" s="3"/>
       <c r="J163" s="10"/>
-      <c r="K163" s="10"/>
-    </row>
-    <row r="164" spans="9:11">
+    </row>
+    <row r="164" spans="9:10">
       <c r="I164" s="3"/>
       <c r="J164" s="10"/>
-      <c r="K164" s="10"/>
-    </row>
-    <row r="165" spans="9:11">
+    </row>
+    <row r="165" spans="9:10">
       <c r="I165" s="3"/>
       <c r="J165" s="10"/>
-      <c r="K165" s="10"/>
-    </row>
-    <row r="166" spans="9:11">
+    </row>
+    <row r="166" spans="9:10">
       <c r="I166" s="3"/>
       <c r="J166" s="10"/>
-      <c r="K166" s="10"/>
-    </row>
-    <row r="167" spans="9:11">
+    </row>
+    <row r="167" spans="9:10">
       <c r="I167" s="3"/>
       <c r="J167" s="10"/>
-      <c r="K167" s="10"/>
-    </row>
-    <row r="168" spans="9:11">
+    </row>
+    <row r="168" spans="9:10">
       <c r="I168" s="3"/>
       <c r="J168" s="10"/>
-      <c r="K168" s="10"/>
-    </row>
-    <row r="169" spans="9:11">
+    </row>
+    <row r="169" spans="9:10">
       <c r="I169" s="3"/>
       <c r="J169" s="10"/>
-      <c r="K169" s="10"/>
-    </row>
-    <row r="170" spans="9:11">
+    </row>
+    <row r="170" spans="9:10">
       <c r="I170" s="3"/>
       <c r="J170" s="10"/>
-      <c r="K170" s="10"/>
-    </row>
-    <row r="171" spans="9:11">
+    </row>
+    <row r="171" spans="9:10">
       <c r="I171" s="3"/>
       <c r="J171" s="10"/>
-      <c r="K171" s="10"/>
-    </row>
-    <row r="172" spans="9:11">
+    </row>
+    <row r="172" spans="9:10">
       <c r="I172" s="3"/>
       <c r="J172" s="10"/>
-      <c r="K172" s="10"/>
-    </row>
-    <row r="173" spans="9:11">
+    </row>
+    <row r="173" spans="9:10">
       <c r="I173" s="3"/>
       <c r="J173" s="10"/>
-      <c r="K173" s="10"/>
-    </row>
-    <row r="174" spans="9:11">
+    </row>
+    <row r="174" spans="9:10">
       <c r="I174" s="3"/>
       <c r="J174" s="10"/>
-      <c r="K174" s="10"/>
-    </row>
-    <row r="175" spans="9:11">
+    </row>
+    <row r="175" spans="9:10">
       <c r="I175" s="3"/>
       <c r="J175" s="10"/>
-      <c r="K175" s="10"/>
-    </row>
-    <row r="176" spans="9:11">
+    </row>
+    <row r="176" spans="9:10">
       <c r="I176" s="3"/>
       <c r="J176" s="10"/>
-      <c r="K176" s="10"/>
-    </row>
-    <row r="177" spans="9:11">
+    </row>
+    <row r="177" spans="9:10">
       <c r="I177" s="3"/>
       <c r="J177" s="10"/>
-      <c r="K177" s="10"/>
-    </row>
-    <row r="178" spans="9:11">
+    </row>
+    <row r="178" spans="9:10">
       <c r="I178" s="3"/>
       <c r="J178" s="10"/>
-      <c r="K178" s="10"/>
-    </row>
-    <row r="179" spans="9:11">
+    </row>
+    <row r="179" spans="9:10">
       <c r="I179" s="3"/>
       <c r="J179" s="10"/>
-      <c r="K179" s="10"/>
-    </row>
-    <row r="180" spans="9:11">
+    </row>
+    <row r="180" spans="9:10">
       <c r="I180" s="3"/>
       <c r="J180" s="10"/>
-      <c r="K180" s="10"/>
-    </row>
-    <row r="181" spans="9:11">
+    </row>
+    <row r="181" spans="9:10">
       <c r="I181" s="3"/>
       <c r="J181" s="10"/>
-      <c r="K181" s="10"/>
-    </row>
-    <row r="182" spans="9:11">
+    </row>
+    <row r="182" spans="9:10">
       <c r="I182" s="3"/>
       <c r="J182" s="10"/>
-      <c r="K182" s="10"/>
-    </row>
-    <row r="183" spans="9:11">
+    </row>
+    <row r="183" spans="9:10">
       <c r="I183" s="3"/>
       <c r="J183" s="10"/>
-      <c r="K183" s="10"/>
-    </row>
-    <row r="184" spans="9:11">
+    </row>
+    <row r="184" spans="9:10">
       <c r="I184" s="3"/>
       <c r="J184" s="10"/>
-      <c r="K184" s="10"/>
-    </row>
-    <row r="185" spans="9:11">
+    </row>
+    <row r="185" spans="9:10">
       <c r="I185" s="3"/>
       <c r="J185" s="10"/>
-      <c r="K185" s="10"/>
-    </row>
-    <row r="186" spans="9:11">
+    </row>
+    <row r="186" spans="9:10">
       <c r="I186" s="3"/>
       <c r="J186" s="10"/>
-      <c r="K186" s="10"/>
-    </row>
-    <row r="187" spans="9:11">
+    </row>
+    <row r="187" spans="9:10">
       <c r="I187" s="3"/>
       <c r="J187" s="10"/>
-      <c r="K187" s="10"/>
-    </row>
-    <row r="188" spans="9:11">
+    </row>
+    <row r="188" spans="9:10">
       <c r="I188" s="3"/>
       <c r="J188" s="10"/>
-      <c r="K188" s="10"/>
-    </row>
-    <row r="189" spans="9:11">
+    </row>
+    <row r="189" spans="9:10">
       <c r="I189" s="3"/>
       <c r="J189" s="10"/>
-      <c r="K189" s="10"/>
-    </row>
-    <row r="190" spans="9:11">
+    </row>
+    <row r="190" spans="9:10">
       <c r="I190" s="3"/>
       <c r="J190" s="10"/>
-      <c r="K190" s="10"/>
-    </row>
-    <row r="191" spans="9:11">
+    </row>
+    <row r="191" spans="9:10">
       <c r="I191" s="3"/>
       <c r="J191" s="10"/>
-      <c r="K191" s="10"/>
-    </row>
-    <row r="192" spans="9:11">
+    </row>
+    <row r="192" spans="9:10">
       <c r="I192" s="3"/>
       <c r="J192" s="10"/>
-      <c r="K192" s="10"/>
-    </row>
-    <row r="193" spans="9:11">
+    </row>
+    <row r="193" spans="9:10">
       <c r="I193" s="3"/>
       <c r="J193" s="10"/>
-      <c r="K193" s="10"/>
-    </row>
-    <row r="194" spans="9:11">
+    </row>
+    <row r="194" spans="9:10">
       <c r="I194" s="3"/>
       <c r="J194" s="10"/>
-      <c r="K194" s="10"/>
-    </row>
-    <row r="195" spans="9:11">
+    </row>
+    <row r="195" spans="9:10">
       <c r="I195" s="3"/>
       <c r="J195" s="10"/>
-      <c r="K195" s="10"/>
-    </row>
-    <row r="196" spans="9:11">
+    </row>
+    <row r="196" spans="9:10">
       <c r="I196" s="3"/>
       <c r="J196" s="10"/>
-      <c r="K196" s="10"/>
-    </row>
-    <row r="197" spans="9:11">
+    </row>
+    <row r="197" spans="9:10">
       <c r="I197" s="3"/>
       <c r="J197" s="10"/>
-      <c r="K197" s="10"/>
-    </row>
-    <row r="198" spans="9:11">
+    </row>
+    <row r="198" spans="9:10">
       <c r="I198" s="3"/>
       <c r="J198" s="10"/>
-      <c r="K198" s="10"/>
-    </row>
-    <row r="199" spans="9:11">
+    </row>
+    <row r="199" spans="9:10">
       <c r="I199" s="3"/>
       <c r="J199" s="10"/>
-      <c r="K199" s="10"/>
-    </row>
-    <row r="200" spans="9:11">
+    </row>
+    <row r="200" spans="9:10">
       <c r="I200" s="3"/>
       <c r="J200" s="10"/>
-      <c r="K200" s="10"/>
-    </row>
-    <row r="201" spans="9:11">
+    </row>
+    <row r="201" spans="9:10">
       <c r="I201" s="3"/>
       <c r="J201" s="10"/>
-      <c r="K201" s="10"/>
-    </row>
-    <row r="202" spans="9:11">
+    </row>
+    <row r="202" spans="9:10">
       <c r="I202" s="3"/>
       <c r="J202" s="10"/>
-      <c r="K202" s="10"/>
-    </row>
-    <row r="203" spans="9:11">
+    </row>
+    <row r="203" spans="9:10">
       <c r="I203" s="3"/>
       <c r="J203" s="10"/>
-      <c r="K203" s="10"/>
-    </row>
-    <row r="204" spans="9:11">
+    </row>
+    <row r="204" spans="9:10">
       <c r="I204" s="3"/>
       <c r="J204" s="10"/>
-      <c r="K204" s="10"/>
-    </row>
-    <row r="205" spans="9:11">
+    </row>
+    <row r="205" spans="9:10">
       <c r="I205" s="3"/>
       <c r="J205" s="10"/>
-      <c r="K205" s="10"/>
-    </row>
-    <row r="206" spans="9:11">
+    </row>
+    <row r="206" spans="9:10">
       <c r="I206" s="3"/>
       <c r="J206" s="10"/>
-      <c r="K206" s="10"/>
-    </row>
-    <row r="207" spans="9:11">
+    </row>
+    <row r="207" spans="9:10">
       <c r="I207" s="3"/>
       <c r="J207" s="10"/>
-      <c r="K207" s="10"/>
-    </row>
-    <row r="208" spans="9:11">
+    </row>
+    <row r="208" spans="9:10">
       <c r="I208" s="3"/>
       <c r="J208" s="10"/>
-      <c r="K208" s="10"/>
-    </row>
-    <row r="209" spans="9:11">
+    </row>
+    <row r="209" spans="9:10">
       <c r="I209" s="3"/>
       <c r="J209" s="10"/>
-      <c r="K209" s="10"/>
-    </row>
-    <row r="210" spans="9:11">
+    </row>
+    <row r="210" spans="9:10">
       <c r="I210" s="3"/>
       <c r="J210" s="10"/>
-      <c r="K210" s="10"/>
-    </row>
-    <row r="211" spans="9:11">
+    </row>
+    <row r="211" spans="9:10">
       <c r="I211" s="3"/>
       <c r="J211" s="10"/>
-      <c r="K211" s="10"/>
-    </row>
-    <row r="212" spans="9:11">
+    </row>
+    <row r="212" spans="9:10">
       <c r="I212" s="3"/>
       <c r="J212" s="10"/>
-      <c r="K212" s="10"/>
-    </row>
-    <row r="213" spans="9:11">
+    </row>
+    <row r="213" spans="9:10">
       <c r="I213" s="3"/>
       <c r="J213" s="10"/>
-      <c r="K213" s="10"/>
-    </row>
-    <row r="214" spans="9:11">
+    </row>
+    <row r="214" spans="9:10">
       <c r="I214" s="3"/>
       <c r="J214" s="10"/>
-      <c r="K214" s="10"/>
-    </row>
-    <row r="215" spans="9:11">
+    </row>
+    <row r="215" spans="9:10">
       <c r="I215" s="3"/>
       <c r="J215" s="10"/>
-      <c r="K215" s="10"/>
-    </row>
-    <row r="216" spans="9:11">
+    </row>
+    <row r="216" spans="9:10">
       <c r="I216" s="3"/>
       <c r="J216" s="10"/>
-      <c r="K216" s="10"/>
-    </row>
-    <row r="217" spans="9:11">
+    </row>
+    <row r="217" spans="9:10">
       <c r="I217" s="3"/>
       <c r="J217" s="10"/>
-      <c r="K217" s="10"/>
-    </row>
-    <row r="218" spans="9:11">
+    </row>
+    <row r="218" spans="9:10">
       <c r="I218" s="3"/>
       <c r="J218" s="10"/>
-      <c r="K218" s="10"/>
-    </row>
-    <row r="219" spans="9:11">
+    </row>
+    <row r="219" spans="9:10">
       <c r="I219" s="3"/>
       <c r="J219" s="10"/>
-      <c r="K219" s="10"/>
-    </row>
-    <row r="220" spans="9:11">
+    </row>
+    <row r="220" spans="9:10">
       <c r="I220" s="3"/>
       <c r="J220" s="10"/>
-      <c r="K220" s="10"/>
-    </row>
-    <row r="221" spans="9:11">
+    </row>
+    <row r="221" spans="9:10">
       <c r="I221" s="3"/>
       <c r="J221" s="10"/>
-      <c r="K221" s="10"/>
-    </row>
-    <row r="222" spans="9:11">
+    </row>
+    <row r="222" spans="9:10">
       <c r="I222" s="3"/>
       <c r="J222" s="10"/>
-      <c r="K222" s="10"/>
-    </row>
-    <row r="223" spans="9:11">
+    </row>
+    <row r="223" spans="9:10">
       <c r="I223" s="3"/>
       <c r="J223" s="10"/>
-      <c r="K223" s="10"/>
-    </row>
-    <row r="224" spans="9:11">
+    </row>
+    <row r="224" spans="9:10">
       <c r="I224" s="3"/>
       <c r="J224" s="10"/>
-      <c r="K224" s="10"/>
-    </row>
-    <row r="225" spans="9:11">
+    </row>
+    <row r="225" spans="9:10">
       <c r="I225" s="3"/>
       <c r="J225" s="10"/>
-      <c r="K225" s="10"/>
-    </row>
-    <row r="226" spans="9:11">
+    </row>
+    <row r="226" spans="9:10">
       <c r="I226" s="3"/>
       <c r="J226" s="10"/>
-      <c r="K226" s="10"/>
-    </row>
-    <row r="227" spans="9:11">
+    </row>
+    <row r="227" spans="9:10">
       <c r="I227" s="3"/>
       <c r="J227" s="10"/>
-      <c r="K227" s="10"/>
-    </row>
-    <row r="228" spans="9:11">
+    </row>
+    <row r="228" spans="9:10">
       <c r="I228" s="3"/>
       <c r="J228" s="10"/>
-      <c r="K228" s="10"/>
-    </row>
-    <row r="229" spans="9:11">
+    </row>
+    <row r="229" spans="9:10">
       <c r="I229" s="3"/>
       <c r="J229" s="10"/>
-      <c r="K229" s="10"/>
-    </row>
-    <row r="230" spans="9:11">
+    </row>
+    <row r="230" spans="9:10">
       <c r="I230" s="3"/>
       <c r="J230" s="10"/>
-      <c r="K230" s="10"/>
-    </row>
-    <row r="231" spans="9:11">
+    </row>
+    <row r="231" spans="9:10">
       <c r="I231" s="3"/>
       <c r="J231" s="10"/>
-      <c r="K231" s="10"/>
-    </row>
-    <row r="232" spans="9:11">
+    </row>
+    <row r="232" spans="9:10">
       <c r="I232" s="3"/>
       <c r="J232" s="10"/>
-      <c r="K232" s="10"/>
-    </row>
-    <row r="233" spans="9:11">
+    </row>
+    <row r="233" spans="9:10">
       <c r="I233" s="3"/>
       <c r="J233" s="10"/>
-      <c r="K233" s="10"/>
-    </row>
-    <row r="234" spans="9:11">
+    </row>
+    <row r="234" spans="9:10">
       <c r="I234" s="3"/>
       <c r="J234" s="10"/>
-      <c r="K234" s="10"/>
-    </row>
-    <row r="235" spans="9:11">
+    </row>
+    <row r="235" spans="9:10">
       <c r="I235" s="3"/>
       <c r="J235" s="10"/>
-      <c r="K235" s="10"/>
-    </row>
-    <row r="236" spans="9:11">
+    </row>
+    <row r="236" spans="9:10">
       <c r="I236" s="3"/>
       <c r="J236" s="10"/>
-      <c r="K236" s="10"/>
-    </row>
-    <row r="237" spans="9:11">
+    </row>
+    <row r="237" spans="9:10">
       <c r="I237" s="3"/>
       <c r="J237" s="10"/>
-      <c r="K237" s="10"/>
-    </row>
-    <row r="238" spans="9:11">
+    </row>
+    <row r="238" spans="9:10">
       <c r="I238" s="3"/>
       <c r="J238" s="10"/>
-      <c r="K238" s="10"/>
-    </row>
-    <row r="239" spans="9:11">
+    </row>
+    <row r="239" spans="9:10">
       <c r="I239" s="3"/>
       <c r="J239" s="10"/>
-      <c r="K239" s="10"/>
-    </row>
-    <row r="240" spans="9:11">
+    </row>
+    <row r="240" spans="9:10">
       <c r="I240" s="3"/>
       <c r="J240" s="10"/>
-      <c r="K240" s="10"/>
-    </row>
-    <row r="241" spans="9:11">
+    </row>
+    <row r="241" spans="9:10">
       <c r="I241" s="3"/>
       <c r="J241" s="10"/>
-      <c r="K241" s="10"/>
-    </row>
-    <row r="242" spans="9:11">
+    </row>
+    <row r="242" spans="9:10">
       <c r="I242" s="3"/>
       <c r="J242" s="10"/>
-      <c r="K242" s="10"/>
-    </row>
-    <row r="243" spans="9:11">
+    </row>
+    <row r="243" spans="9:10">
       <c r="I243" s="3"/>
       <c r="J243" s="10"/>
-      <c r="K243" s="10"/>
-    </row>
-    <row r="244" spans="9:11">
+    </row>
+    <row r="244" spans="9:10">
       <c r="I244" s="3"/>
       <c r="J244" s="10"/>
-      <c r="K244" s="10"/>
-    </row>
-    <row r="245" spans="9:11">
+    </row>
+    <row r="245" spans="9:10">
       <c r="I245" s="3"/>
       <c r="J245" s="10"/>
-      <c r="K245" s="10"/>
-    </row>
-    <row r="246" spans="9:11">
+    </row>
+    <row r="246" spans="9:10">
       <c r="I246" s="3"/>
       <c r="J246" s="10"/>
-      <c r="K246" s="10"/>
-    </row>
-    <row r="247" spans="9:11">
+    </row>
+    <row r="247" spans="9:10">
       <c r="I247" s="3"/>
       <c r="J247" s="10"/>
-      <c r="K247" s="10"/>
-    </row>
-    <row r="248" spans="9:11">
+    </row>
+    <row r="248" spans="9:10">
       <c r="I248" s="3"/>
       <c r="J248" s="10"/>
-      <c r="K248" s="10"/>
-    </row>
-    <row r="249" spans="9:11">
+    </row>
+    <row r="249" spans="9:10">
       <c r="I249" s="3"/>
       <c r="J249" s="10"/>
-      <c r="K249" s="10"/>
-    </row>
-    <row r="250" spans="9:11">
+    </row>
+    <row r="250" spans="9:10">
       <c r="I250" s="3"/>
       <c r="J250" s="10"/>
-      <c r="K250" s="10"/>
-    </row>
-    <row r="251" spans="9:11">
+    </row>
+    <row r="251" spans="9:10">
       <c r="I251" s="3"/>
       <c r="J251" s="10"/>
-      <c r="K251" s="10"/>
-    </row>
-    <row r="252" spans="9:11">
+    </row>
+    <row r="252" spans="9:10">
       <c r="I252" s="3"/>
       <c r="J252" s="10"/>
-      <c r="K252" s="10"/>
-    </row>
-    <row r="253" spans="9:11">
+    </row>
+    <row r="253" spans="9:10">
       <c r="I253" s="3"/>
       <c r="J253" s="10"/>
-      <c r="K253" s="10"/>
-    </row>
-    <row r="254" spans="9:11">
+    </row>
+    <row r="254" spans="9:10">
       <c r="I254" s="3"/>
       <c r="J254" s="10"/>
-      <c r="K254" s="10"/>
-    </row>
-    <row r="255" spans="9:11">
+    </row>
+    <row r="255" spans="9:10">
       <c r="I255" s="3"/>
       <c r="J255" s="10"/>
-      <c r="K255" s="10"/>
-    </row>
-    <row r="256" spans="9:11">
+    </row>
+    <row r="256" spans="9:10">
       <c r="I256" s="3"/>
       <c r="J256" s="10"/>
-      <c r="K256" s="10"/>
-    </row>
-    <row r="257" spans="9:11">
+    </row>
+    <row r="257" spans="9:10">
       <c r="I257" s="3"/>
       <c r="J257" s="10"/>
-      <c r="K257" s="10"/>
-    </row>
-    <row r="258" spans="9:11">
+    </row>
+    <row r="258" spans="9:10">
       <c r="I258" s="3"/>
       <c r="J258" s="10"/>
-      <c r="K258" s="10"/>
-    </row>
-    <row r="259" spans="9:11">
+    </row>
+    <row r="259" spans="9:10">
       <c r="I259" s="3"/>
       <c r="J259" s="10"/>
-      <c r="K259" s="10"/>
-    </row>
-    <row r="260" spans="9:11">
+    </row>
+    <row r="260" spans="9:10">
       <c r="I260" s="3"/>
       <c r="J260" s="10"/>
-      <c r="K260" s="10"/>
-    </row>
-    <row r="261" spans="9:11">
+    </row>
+    <row r="261" spans="9:10">
       <c r="I261" s="3"/>
       <c r="J261" s="10"/>
-      <c r="K261" s="10"/>
-    </row>
-    <row r="262" spans="9:11">
+    </row>
+    <row r="262" spans="9:10">
       <c r="I262" s="3"/>
       <c r="J262" s="10"/>
-      <c r="K262" s="10"/>
-    </row>
-    <row r="263" spans="9:11">
+    </row>
+    <row r="263" spans="9:10">
       <c r="I263" s="3"/>
       <c r="J263" s="10"/>
-      <c r="K263" s="10"/>
-    </row>
-    <row r="264" spans="9:11">
+    </row>
+    <row r="264" spans="9:10">
       <c r="I264" s="3"/>
       <c r="J264" s="10"/>
-      <c r="K264" s="10"/>
-    </row>
-    <row r="265" spans="9:11">
+    </row>
+    <row r="265" spans="9:10">
       <c r="I265" s="3"/>
       <c r="J265" s="10"/>
-      <c r="K265" s="10"/>
-    </row>
-    <row r="266" spans="9:11">
+    </row>
+    <row r="266" spans="9:10">
       <c r="I266" s="3"/>
       <c r="J266" s="10"/>
-      <c r="K266" s="10"/>
-    </row>
-    <row r="267" spans="9:11">
+    </row>
+    <row r="267" spans="9:10">
       <c r="I267" s="3"/>
       <c r="J267" s="10"/>
-      <c r="K267" s="10"/>
-    </row>
-    <row r="268" spans="9:11">
+    </row>
+    <row r="268" spans="9:10">
       <c r="I268" s="3"/>
       <c r="J268" s="10"/>
-      <c r="K268" s="10"/>
-    </row>
-    <row r="269" spans="9:11">
+    </row>
+    <row r="269" spans="9:10">
       <c r="I269" s="3"/>
       <c r="J269" s="10"/>
-      <c r="K269" s="10"/>
-    </row>
-    <row r="270" spans="9:11">
+    </row>
+    <row r="270" spans="9:10">
       <c r="I270" s="3"/>
       <c r="J270" s="10"/>
-      <c r="K270" s="10"/>
-    </row>
-    <row r="271" spans="9:11">
+    </row>
+    <row r="271" spans="9:10">
       <c r="I271" s="3"/>
       <c r="J271" s="10"/>
-      <c r="K271" s="10"/>
-    </row>
-    <row r="272" spans="9:11">
+    </row>
+    <row r="272" spans="9:10">
       <c r="I272" s="3"/>
       <c r="J272" s="10"/>
-      <c r="K272" s="10"/>
-    </row>
-    <row r="273" spans="9:11">
+    </row>
+    <row r="273" spans="9:10">
       <c r="I273" s="3"/>
       <c r="J273" s="10"/>
-      <c r="K273" s="10"/>
-    </row>
-    <row r="274" spans="9:11">
+    </row>
+    <row r="274" spans="9:10">
       <c r="I274" s="3"/>
       <c r="J274" s="10"/>
-      <c r="K274" s="10"/>
-    </row>
-    <row r="275" spans="9:11">
+    </row>
+    <row r="275" spans="9:10">
       <c r="I275" s="3"/>
       <c r="J275" s="10"/>
-      <c r="K275" s="10"/>
-    </row>
-    <row r="276" spans="9:11">
+    </row>
+    <row r="276" spans="9:10">
       <c r="I276" s="3"/>
       <c r="J276" s="10"/>
-      <c r="K276" s="10"/>
-    </row>
-    <row r="277" spans="9:11">
+    </row>
+    <row r="277" spans="9:10">
       <c r="I277" s="3"/>
       <c r="J277" s="10"/>
-      <c r="K277" s="10"/>
-    </row>
-    <row r="278" spans="9:11">
+    </row>
+    <row r="278" spans="9:10">
       <c r="I278" s="3"/>
       <c r="J278" s="10"/>
-      <c r="K278" s="10"/>
-    </row>
-    <row r="279" spans="9:11">
+    </row>
+    <row r="279" spans="9:10">
       <c r="I279" s="3"/>
       <c r="J279" s="10"/>
-      <c r="K279" s="10"/>
-    </row>
-    <row r="280" spans="9:11">
+    </row>
+    <row r="280" spans="9:10">
       <c r="I280" s="3"/>
       <c r="J280" s="10"/>
-      <c r="K280" s="10"/>
-    </row>
-    <row r="281" spans="9:11">
+    </row>
+    <row r="281" spans="9:10">
       <c r="I281" s="3"/>
       <c r="J281" s="10"/>
-      <c r="K281" s="10"/>
-    </row>
-    <row r="282" spans="9:11">
+    </row>
+    <row r="282" spans="9:10">
       <c r="I282" s="3"/>
       <c r="J282" s="10"/>
-      <c r="K282" s="10"/>
-    </row>
-    <row r="283" spans="9:11">
+    </row>
+    <row r="283" spans="9:10">
       <c r="I283" s="3"/>
       <c r="J283" s="10"/>
-      <c r="K283" s="10"/>
-    </row>
-    <row r="284" spans="9:11">
+    </row>
+    <row r="284" spans="9:10">
       <c r="I284" s="3"/>
       <c r="J284" s="10"/>
-      <c r="K284" s="10"/>
-    </row>
-    <row r="285" spans="9:11">
+    </row>
+    <row r="285" spans="9:10">
       <c r="I285" s="3"/>
       <c r="J285" s="10"/>
-      <c r="K285" s="10"/>
-    </row>
-    <row r="286" spans="9:11">
+    </row>
+    <row r="286" spans="9:10">
       <c r="I286" s="3"/>
       <c r="J286" s="10"/>
-      <c r="K286" s="10"/>
-    </row>
-    <row r="287" spans="9:11">
+    </row>
+    <row r="287" spans="9:10">
       <c r="I287" s="3"/>
       <c r="J287" s="10"/>
-      <c r="K287" s="10"/>
-    </row>
-    <row r="288" spans="9:11">
+    </row>
+    <row r="288" spans="9:10">
       <c r="I288" s="3"/>
       <c r="J288" s="10"/>
-      <c r="K288" s="10"/>
-    </row>
-    <row r="289" spans="9:11">
+    </row>
+    <row r="289" spans="9:10">
       <c r="I289" s="3"/>
       <c r="J289" s="10"/>
-      <c r="K289" s="10"/>
-    </row>
-    <row r="290" spans="9:11">
+    </row>
+    <row r="290" spans="9:10">
       <c r="I290" s="3"/>
       <c r="J290" s="10"/>
-      <c r="K290" s="10"/>
-    </row>
-    <row r="291" spans="9:11">
+    </row>
+    <row r="291" spans="9:10">
       <c r="I291" s="3"/>
       <c r="J291" s="10"/>
-      <c r="K291" s="10"/>
-    </row>
-    <row r="292" spans="9:11">
+    </row>
+    <row r="292" spans="9:10">
       <c r="I292" s="3"/>
       <c r="J292" s="10"/>
-      <c r="K292" s="10"/>
-    </row>
-    <row r="293" spans="9:11">
+    </row>
+    <row r="293" spans="9:10">
       <c r="I293" s="3"/>
       <c r="J293" s="10"/>
-      <c r="K293" s="10"/>
-    </row>
-    <row r="294" spans="9:11">
+    </row>
+    <row r="294" spans="9:10">
       <c r="I294" s="3"/>
       <c r="J294" s="10"/>
-      <c r="K294" s="10"/>
-    </row>
-    <row r="295" spans="9:11">
+    </row>
+    <row r="295" spans="9:10">
       <c r="I295" s="3"/>
       <c r="J295" s="10"/>
-      <c r="K295" s="10"/>
-    </row>
-    <row r="296" spans="9:11">
+    </row>
+    <row r="296" spans="9:10">
       <c r="I296" s="3"/>
       <c r="J296" s="10"/>
-      <c r="K296" s="10"/>
-    </row>
-    <row r="297" spans="9:11">
+    </row>
+    <row r="297" spans="9:10">
       <c r="I297" s="3"/>
       <c r="J297" s="10"/>
-      <c r="K297" s="10"/>
-    </row>
-    <row r="298" spans="9:11">
+    </row>
+    <row r="298" spans="9:10">
       <c r="I298" s="3"/>
       <c r="J298" s="10"/>
-      <c r="K298" s="10"/>
-    </row>
-    <row r="299" spans="9:11">
+    </row>
+    <row r="299" spans="9:10">
       <c r="I299" s="3"/>
       <c r="J299" s="10"/>
-      <c r="K299" s="10"/>
-    </row>
-    <row r="300" spans="9:11">
+    </row>
+    <row r="300" spans="9:10">
       <c r="I300" s="3"/>
       <c r="J300" s="10"/>
-      <c r="K300" s="10"/>
-    </row>
-    <row r="301" spans="9:11">
+    </row>
+    <row r="301" spans="9:10">
       <c r="I301" s="3"/>
       <c r="J301" s="10"/>
-      <c r="K301" s="10"/>
-    </row>
-    <row r="302" spans="9:11">
+    </row>
+    <row r="302" spans="9:10">
       <c r="I302" s="3"/>
       <c r="J302" s="10"/>
-      <c r="K302" s="10"/>
-    </row>
-    <row r="303" spans="9:11">
+    </row>
+    <row r="303" spans="9:10">
       <c r="I303" s="3"/>
       <c r="J303" s="10"/>
-      <c r="K303" s="10"/>
-    </row>
-    <row r="304" spans="9:11">
+    </row>
+    <row r="304" spans="9:10">
       <c r="I304" s="3"/>
       <c r="J304" s="10"/>
-      <c r="K304" s="10"/>
-    </row>
-    <row r="305" spans="9:11">
+    </row>
+    <row r="305" spans="9:10">
       <c r="I305" s="3"/>
       <c r="J305" s="10"/>
-      <c r="K305" s="10"/>
-    </row>
-    <row r="306" spans="9:11">
+    </row>
+    <row r="306" spans="9:10">
       <c r="I306" s="3"/>
       <c r="J306" s="10"/>
-      <c r="K306" s="10"/>
-    </row>
-    <row r="307" spans="9:11">
+    </row>
+    <row r="307" spans="9:10">
       <c r="I307" s="3"/>
       <c r="J307" s="10"/>
-      <c r="K307" s="10"/>
-    </row>
-    <row r="308" spans="9:11">
+    </row>
+    <row r="308" spans="9:10">
       <c r="I308" s="3"/>
       <c r="J308" s="10"/>
-      <c r="K308" s="10"/>
-    </row>
-    <row r="309" spans="9:11">
+    </row>
+    <row r="309" spans="9:10">
       <c r="I309" s="3"/>
       <c r="J309" s="10"/>
-      <c r="K309" s="10"/>
-    </row>
-    <row r="310" spans="9:11">
+    </row>
+    <row r="310" spans="9:10">
       <c r="I310" s="3"/>
       <c r="J310" s="10"/>
-      <c r="K310" s="10"/>
-    </row>
-    <row r="311" spans="9:11">
+    </row>
+    <row r="311" spans="9:10">
       <c r="I311" s="3"/>
       <c r="J311" s="10"/>
-      <c r="K311" s="10"/>
-    </row>
-    <row r="312" spans="9:11">
+    </row>
+    <row r="312" spans="9:10">
       <c r="I312" s="3"/>
       <c r="J312" s="10"/>
-      <c r="K312" s="10"/>
-    </row>
-    <row r="313" spans="9:11">
+    </row>
+    <row r="313" spans="9:10">
       <c r="I313" s="3"/>
       <c r="J313" s="10"/>
-      <c r="K313" s="10"/>
-    </row>
-    <row r="314" spans="9:11">
+    </row>
+    <row r="314" spans="9:10">
       <c r="I314" s="3"/>
       <c r="J314" s="10"/>
-      <c r="K314" s="10"/>
-    </row>
-    <row r="315" spans="9:11">
+    </row>
+    <row r="315" spans="9:10">
       <c r="I315" s="3"/>
       <c r="J315" s="10"/>
-      <c r="K315" s="10"/>
-    </row>
-    <row r="316" spans="9:11">
+    </row>
+    <row r="316" spans="9:10">
       <c r="I316" s="3"/>
       <c r="J316" s="10"/>
-      <c r="K316" s="10"/>
-    </row>
-    <row r="317" spans="9:11">
+    </row>
+    <row r="317" spans="9:10">
       <c r="I317" s="3"/>
       <c r="J317" s="10"/>
-      <c r="K317" s="10"/>
-    </row>
-    <row r="318" spans="9:11">
+    </row>
+    <row r="318" spans="9:10">
       <c r="I318" s="3"/>
       <c r="J318" s="10"/>
-      <c r="K318" s="10"/>
-    </row>
-    <row r="319" spans="9:11">
+    </row>
+    <row r="319" spans="9:10">
       <c r="I319" s="3"/>
       <c r="J319" s="10"/>
-      <c r="K319" s="10"/>
-    </row>
-    <row r="320" spans="9:11">
+    </row>
+    <row r="320" spans="9:10">
       <c r="I320" s="3"/>
       <c r="J320" s="10"/>
-      <c r="K320" s="10"/>
-    </row>
-    <row r="321" spans="9:11">
+    </row>
+    <row r="321" spans="9:10">
       <c r="I321" s="3"/>
       <c r="J321" s="10"/>
-      <c r="K321" s="10"/>
-    </row>
-    <row r="322" spans="9:11">
+    </row>
+    <row r="322" spans="9:10">
       <c r="I322" s="3"/>
       <c r="J322" s="10"/>
-      <c r="K322" s="10"/>
-    </row>
-    <row r="323" spans="9:11">
+    </row>
+    <row r="323" spans="9:10">
       <c r="I323" s="3"/>
       <c r="J323" s="10"/>
-      <c r="K323" s="10"/>
-    </row>
-    <row r="324" spans="9:11">
+    </row>
+    <row r="324" spans="9:10">
       <c r="I324" s="3"/>
       <c r="J324" s="10"/>
-      <c r="K324" s="10"/>
-    </row>
-    <row r="325" spans="9:11">
+    </row>
+    <row r="325" spans="9:10">
       <c r="I325" s="3"/>
       <c r="J325" s="10"/>
-      <c r="K325" s="10"/>
-    </row>
-    <row r="326" spans="9:11">
+    </row>
+    <row r="326" spans="9:10">
       <c r="I326" s="3"/>
       <c r="J326" s="10"/>
-      <c r="K326" s="10"/>
-    </row>
-    <row r="327" spans="9:11">
+    </row>
+    <row r="327" spans="9:10">
       <c r="I327" s="3"/>
       <c r="J327" s="10"/>
-      <c r="K327" s="10"/>
-    </row>
-    <row r="328" spans="9:11">
+    </row>
+    <row r="328" spans="9:10">
       <c r="I328" s="3"/>
       <c r="J328" s="10"/>
-      <c r="K328" s="10"/>
-    </row>
-    <row r="329" spans="9:11">
+    </row>
+    <row r="329" spans="9:10">
       <c r="I329" s="3"/>
       <c r="J329" s="10"/>
-      <c r="K329" s="10"/>
-    </row>
-    <row r="330" spans="9:11">
+    </row>
+    <row r="330" spans="9:10">
       <c r="I330" s="3"/>
       <c r="J330" s="10"/>
-      <c r="K330" s="10"/>
-    </row>
-    <row r="331" spans="9:11">
+    </row>
+    <row r="331" spans="9:10">
       <c r="I331" s="3"/>
       <c r="J331" s="10"/>
-      <c r="K331" s="10"/>
-    </row>
-    <row r="332" spans="9:11">
+    </row>
+    <row r="332" spans="9:10">
       <c r="I332" s="3"/>
       <c r="J332" s="10"/>
-      <c r="K332" s="10"/>
-    </row>
-    <row r="333" spans="9:11">
+    </row>
+    <row r="333" spans="9:10">
       <c r="I333" s="3"/>
       <c r="J333" s="10"/>
-      <c r="K333" s="10"/>
-    </row>
-    <row r="334" spans="9:11">
+    </row>
+    <row r="334" spans="9:10">
       <c r="I334" s="3"/>
       <c r="J334" s="10"/>
-      <c r="K334" s="10"/>
-    </row>
-    <row r="335" spans="9:11">
+    </row>
+    <row r="335" spans="9:10">
       <c r="I335" s="3"/>
       <c r="J335" s="10"/>
-      <c r="K335" s="10"/>
-    </row>
-    <row r="336" spans="9:11">
+    </row>
+    <row r="336" spans="9:10">
       <c r="I336" s="3"/>
       <c r="J336" s="10"/>
-      <c r="K336" s="10"/>
-    </row>
-    <row r="337" spans="9:11">
+    </row>
+    <row r="337" spans="9:10">
       <c r="I337" s="3"/>
       <c r="J337" s="10"/>
-      <c r="K337" s="10"/>
-    </row>
-    <row r="338" spans="9:11">
+    </row>
+    <row r="338" spans="9:10">
       <c r="I338" s="3"/>
       <c r="J338" s="10"/>
-      <c r="K338" s="10"/>
-    </row>
-    <row r="339" spans="9:11">
+    </row>
+    <row r="339" spans="9:10">
       <c r="I339" s="3"/>
       <c r="J339" s="10"/>
-      <c r="K339" s="10"/>
-    </row>
-    <row r="340" spans="9:11">
+    </row>
+    <row r="340" spans="9:10">
       <c r="I340" s="3"/>
       <c r="J340" s="10"/>
-      <c r="K340" s="10"/>
-    </row>
-    <row r="341" spans="9:11">
+    </row>
+    <row r="341" spans="9:10">
       <c r="I341" s="3"/>
       <c r="J341" s="10"/>
-      <c r="K341" s="10"/>
-    </row>
-    <row r="342" spans="9:11">
+    </row>
+    <row r="342" spans="9:10">
       <c r="I342" s="3"/>
       <c r="J342" s="10"/>
-      <c r="K342" s="10"/>
-    </row>
-    <row r="343" spans="9:11">
+    </row>
+    <row r="343" spans="9:10">
       <c r="I343" s="3"/>
       <c r="J343" s="10"/>
-      <c r="K343" s="10"/>
-    </row>
-    <row r="344" spans="9:11">
+    </row>
+    <row r="344" spans="9:10">
       <c r="I344" s="3"/>
       <c r="J344" s="10"/>
-      <c r="K344" s="10"/>
-    </row>
-    <row r="345" spans="9:11">
+    </row>
+    <row r="345" spans="9:10">
       <c r="I345" s="3"/>
       <c r="J345" s="10"/>
-      <c r="K345" s="10"/>
-    </row>
-    <row r="346" spans="9:11">
+    </row>
+    <row r="346" spans="9:10">
       <c r="I346" s="3"/>
       <c r="J346" s="10"/>
-      <c r="K346" s="10"/>
-    </row>
-    <row r="347" spans="9:11">
+    </row>
+    <row r="347" spans="9:10">
       <c r="I347" s="3"/>
       <c r="J347" s="10"/>
-      <c r="K347" s="10"/>
-    </row>
-    <row r="348" spans="9:11">
+    </row>
+    <row r="348" spans="9:10">
       <c r="I348" s="3"/>
       <c r="J348" s="10"/>
-      <c r="K348" s="10"/>
-    </row>
-    <row r="349" spans="9:11">
+    </row>
+    <row r="349" spans="9:10">
       <c r="I349" s="3"/>
       <c r="J349" s="10"/>
-      <c r="K349" s="10"/>
-    </row>
-    <row r="350" spans="9:11">
+    </row>
+    <row r="350" spans="9:10">
       <c r="I350" s="3"/>
       <c r="J350" s="10"/>
-      <c r="K350" s="10"/>
-    </row>
-    <row r="351" spans="9:11">
+    </row>
+    <row r="351" spans="9:10">
       <c r="I351" s="3"/>
       <c r="J351" s="10"/>
-      <c r="K351" s="10"/>
-    </row>
-    <row r="352" spans="9:11">
+    </row>
+    <row r="352" spans="9:10">
       <c r="I352" s="3"/>
       <c r="J352" s="10"/>
-      <c r="K352" s="10"/>
-    </row>
-    <row r="353" spans="9:11">
+    </row>
+    <row r="353" spans="9:10">
       <c r="I353" s="3"/>
       <c r="J353" s="10"/>
-      <c r="K353" s="10"/>
-    </row>
-    <row r="354" spans="9:11">
+    </row>
+    <row r="354" spans="9:10">
       <c r="I354" s="3"/>
       <c r="J354" s="10"/>
-      <c r="K354" s="10"/>
-    </row>
-    <row r="355" spans="9:11">
+    </row>
+    <row r="355" spans="9:10">
       <c r="I355" s="3"/>
       <c r="J355" s="10"/>
-      <c r="K355" s="10"/>
-    </row>
-    <row r="356" spans="9:11">
+    </row>
+    <row r="356" spans="9:10">
       <c r="I356" s="3"/>
       <c r="J356" s="10"/>
-      <c r="K356" s="10"/>
-    </row>
-    <row r="357" spans="9:11">
+    </row>
+    <row r="357" spans="9:10">
       <c r="I357" s="3"/>
       <c r="J357" s="10"/>
-      <c r="K357" s="10"/>
-    </row>
-    <row r="358" spans="9:11">
+    </row>
+    <row r="358" spans="9:10">
       <c r="I358" s="3"/>
       <c r="J358" s="10"/>
-      <c r="K358" s="10"/>
-    </row>
-    <row r="359" spans="9:11">
+    </row>
+    <row r="359" spans="9:10">
       <c r="I359" s="3"/>
       <c r="J359" s="10"/>
-      <c r="K359" s="10"/>
-    </row>
-    <row r="360" spans="9:11">
+    </row>
+    <row r="360" spans="9:10">
       <c r="I360" s="3"/>
       <c r="J360" s="10"/>
-      <c r="K360" s="10"/>
-    </row>
-    <row r="361" spans="9:11">
+    </row>
+    <row r="361" spans="9:10">
       <c r="I361" s="3"/>
       <c r="J361" s="10"/>
-      <c r="K361" s="10"/>
-    </row>
-    <row r="362" spans="9:11">
+    </row>
+    <row r="362" spans="9:10">
       <c r="I362" s="3"/>
       <c r="J362" s="10"/>
-      <c r="K362" s="10"/>
-    </row>
-    <row r="363" spans="9:11">
+    </row>
+    <row r="363" spans="9:10">
       <c r="I363" s="3"/>
       <c r="J363" s="10"/>
-      <c r="K363" s="10"/>
-    </row>
-    <row r="364" spans="9:11">
+    </row>
+    <row r="364" spans="9:10">
       <c r="I364" s="3"/>
       <c r="J364" s="10"/>
-      <c r="K364" s="10"/>
-    </row>
-    <row r="365" spans="9:11">
+    </row>
+    <row r="365" spans="9:10">
       <c r="I365" s="3"/>
       <c r="J365" s="10"/>
-      <c r="K365" s="10"/>
-    </row>
-    <row r="366" spans="9:11">
+    </row>
+    <row r="366" spans="9:10">
       <c r="I366" s="3"/>
       <c r="J366" s="10"/>
-      <c r="K366" s="10"/>
-    </row>
-    <row r="367" spans="9:11">
+    </row>
+    <row r="367" spans="9:10">
       <c r="I367" s="3"/>
       <c r="J367" s="10"/>
-      <c r="K367" s="10"/>
-    </row>
-    <row r="368" spans="9:11">
+    </row>
+    <row r="368" spans="9:10">
       <c r="I368" s="3"/>
       <c r="J368" s="10"/>
-      <c r="K368" s="10"/>
-    </row>
-    <row r="369" spans="9:11">
+    </row>
+    <row r="369" spans="9:10">
       <c r="I369" s="3"/>
       <c r="J369" s="10"/>
-      <c r="K369" s="10"/>
-    </row>
-    <row r="370" spans="9:11">
+    </row>
+    <row r="370" spans="9:10">
       <c r="I370" s="3"/>
       <c r="J370" s="10"/>
-      <c r="K370" s="10"/>
-    </row>
-    <row r="371" spans="9:11">
+    </row>
+    <row r="371" spans="9:10">
       <c r="I371" s="3"/>
       <c r="J371" s="10"/>
-      <c r="K371" s="10"/>
-    </row>
-    <row r="372" spans="9:11">
+    </row>
+    <row r="372" spans="9:10">
       <c r="I372" s="3"/>
       <c r="J372" s="10"/>
-      <c r="K372" s="10"/>
-    </row>
-    <row r="373" spans="9:11">
+    </row>
+    <row r="373" spans="9:10">
       <c r="I373" s="3"/>
       <c r="J373" s="10"/>
-      <c r="K373" s="10"/>
-    </row>
-    <row r="374" spans="9:11">
+    </row>
+    <row r="374" spans="9:10">
       <c r="I374" s="3"/>
       <c r="J374" s="10"/>
-      <c r="K374" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="R1:S1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0"/>
@@ -17515,4 +17174,139 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:1" ht="17">
+      <c r="A1" s="16" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="17">
+      <c r="A2" s="16" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="17">
+      <c r="A3" s="16" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="17">
+      <c r="A5" s="16" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="17">
+      <c r="A6" s="16" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="17">
+      <c r="A7" s="16" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="17">
+      <c r="A8" s="16" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="17">
+      <c r="A9" s="16" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="17">
+      <c r="A10" s="16" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="17">
+      <c r="A11" s="16" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="17">
+      <c r="A12" s="16" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="17">
+      <c r="A13" s="16" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="17">
+      <c r="A14" s="16" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="17">
+      <c r="A15" s="16" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="17">
+      <c r="A16" s="16" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="17">
+      <c r="A17" s="16" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="17">
+      <c r="A18" s="16" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="17">
+      <c r="A19" s="16" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="17">
+      <c r="A20" s="16" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" ht="17">
+      <c r="A22" s="16" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" ht="17">
+      <c r="A24" s="16" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" t="s">
+        <v>330</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>